<commit_message>
commit van fixed dataset
</commit_message>
<xml_diff>
--- a/bandcamp_januari_01-02-2017.xlsx
+++ b/bandcamp_januari_01-02-2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomruette/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomruette/git/bandcamp_belgium/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$216</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="513">
   <si>
     <t>artist</t>
   </si>
@@ -996,6 +996,579 @@
   </si>
   <si>
     <t>https://autumna.bandcamp.com/album/afterthought-ep</t>
+  </si>
+  <si>
+    <t>Rock 'n Load Concerts</t>
+  </si>
+  <si>
+    <t>Aalst, Belgium</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>https://rocknloadconcerts.bandcamp.com/album/2017</t>
+  </si>
+  <si>
+    <t>De Groote-Faes Duo</t>
+  </si>
+  <si>
+    <t>Symphony for 2 Little Boys</t>
+  </si>
+  <si>
+    <t>https://degroote-faesduo.bandcamp.com/album/symphony-for-2-little-boys</t>
+  </si>
+  <si>
+    <t>Morgen Wurde</t>
+  </si>
+  <si>
+    <t>Letzten Endes Remixes</t>
+  </si>
+  <si>
+    <t>https://stilll-off.bandcamp.com/album/letzten-endes-remixes</t>
+  </si>
+  <si>
+    <t>RARI</t>
+  </si>
+  <si>
+    <t>I'm Listening Now</t>
+  </si>
+  <si>
+    <t>https://rari.bandcamp.com/album/im-listening-now</t>
+  </si>
+  <si>
+    <t>Haos</t>
+  </si>
+  <si>
+    <t>First Blossoms</t>
+  </si>
+  <si>
+    <t>https://haos.bandcamp.com/album/first-blossoms</t>
+  </si>
+  <si>
+    <t>Mr. Neige</t>
+  </si>
+  <si>
+    <t>A new synth for Mr. Neige</t>
+  </si>
+  <si>
+    <t>https://mrneige.bandcamp.com/album/a-new-synth-for-mr-neige</t>
+  </si>
+  <si>
+    <t>FRANQ</t>
+  </si>
+  <si>
+    <t>Anxious States EP</t>
+  </si>
+  <si>
+    <t>https://franqsmusic.bandcamp.com/album/anxious-states-ep</t>
+  </si>
+  <si>
+    <t>René Schier</t>
+  </si>
+  <si>
+    <t>Zazen</t>
+  </si>
+  <si>
+    <t>http://urbanwavesrecords.com/album/zazen</t>
+  </si>
+  <si>
+    <t>Urban Waves Records</t>
+  </si>
+  <si>
+    <t>PERRON ZES</t>
+  </si>
+  <si>
+    <t>PERRON ZES 1 YEAR COMPILATION</t>
+  </si>
+  <si>
+    <t>https://perronzes.bandcamp.com/album/perron-zes-1-year-compilation</t>
+  </si>
+  <si>
+    <t>Maître Patatus</t>
+  </si>
+  <si>
+    <t>Sans Titre 1</t>
+  </si>
+  <si>
+    <t>https://maitrepatatus.bandcamp.com/album/sans-titre-1</t>
+  </si>
+  <si>
+    <t>Animal Youth</t>
+  </si>
+  <si>
+    <t>YOUTH</t>
+  </si>
+  <si>
+    <t>https://animalyouth.bandcamp.com/album/youth</t>
+  </si>
+  <si>
+    <t>Aslan</t>
+  </si>
+  <si>
+    <t>Ørsted</t>
+  </si>
+  <si>
+    <t>https://aslan1.bandcamp.com/album/rsted</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>INDIA BRUT</t>
+  </si>
+  <si>
+    <t>https://roughtape.bandcamp.com/album/india-brut</t>
+  </si>
+  <si>
+    <t>ROUGH TAPE</t>
+  </si>
+  <si>
+    <t>Leo Hishida</t>
+  </si>
+  <si>
+    <t>Sunny Day in Brussels</t>
+  </si>
+  <si>
+    <t>https://leohishida.bandcamp.com/album/sunny-day-in-brussels</t>
+  </si>
+  <si>
+    <t>Moonai People</t>
+  </si>
+  <si>
+    <t>On a Sunday</t>
+  </si>
+  <si>
+    <t>https://moonaipeople.bandcamp.com/album/on-a-sunday</t>
+  </si>
+  <si>
+    <t>Zonen met vaders</t>
+  </si>
+  <si>
+    <t>Open &amp; dicht</t>
+  </si>
+  <si>
+    <t>https://zonenmetvaders.bandcamp.com/album/open-dicht</t>
+  </si>
+  <si>
+    <t>We Play House Recordings</t>
+  </si>
+  <si>
+    <t>WPH TEN​-​5 Reggie Dokes E​.​P.</t>
+  </si>
+  <si>
+    <t>https://weplayhouserecordings.bandcamp.com/album/wph-ten-5-reggie-dokes-e-p</t>
+  </si>
+  <si>
+    <t>KRANKLAND</t>
+  </si>
+  <si>
+    <t>Dirty Covers - Bedroom Mixtape</t>
+  </si>
+  <si>
+    <t>https://krankland.bandcamp.com/album/dirty-covers-bedroom-mixtape</t>
+  </si>
+  <si>
+    <t>BOTRAMDUUZE</t>
+  </si>
+  <si>
+    <t>RELAXATION &amp; MEDITATION</t>
+  </si>
+  <si>
+    <t>https://botramduuze.bandcamp.com/album/relaxation-meditation</t>
+  </si>
+  <si>
+    <t>Traumatic</t>
+  </si>
+  <si>
+    <t>Xaero &amp; Mel Agony - Lies And Fables (Remixes)</t>
+  </si>
+  <si>
+    <t>https://traumatic.bandcamp.com/album/xaero-mel-agony-lies-and-fables-remixes</t>
+  </si>
+  <si>
+    <t>wim</t>
+  </si>
+  <si>
+    <t>Grobbendonk, Belgium</t>
+  </si>
+  <si>
+    <t>Pardeçu</t>
+  </si>
+  <si>
+    <t>Kruibeke, Belgium</t>
+  </si>
+  <si>
+    <t>Mother Tree</t>
+  </si>
+  <si>
+    <t>https://pardecu.bandcamp.com/album/mother-tree</t>
+  </si>
+  <si>
+    <t>LTGL</t>
+  </si>
+  <si>
+    <t>Leuven, Belgium</t>
+  </si>
+  <si>
+    <t>Splatter Ep [TNGRM014]</t>
+  </si>
+  <si>
+    <t>https://tangramrecords.bandcamp.com/album/splatter-ep-tngrm014</t>
+  </si>
+  <si>
+    <t>Tangram Records</t>
+  </si>
+  <si>
+    <t>Etherik</t>
+  </si>
+  <si>
+    <t>Borderless</t>
+  </si>
+  <si>
+    <t>https://etherik.bandcamp.com/album/borderless</t>
+  </si>
+  <si>
+    <t>Josly Meso</t>
+  </si>
+  <si>
+    <t>Liedekerke, Belgium</t>
+  </si>
+  <si>
+    <t>Naked EP</t>
+  </si>
+  <si>
+    <t>https://joslymeso.bandcamp.com/album/naked-ep</t>
+  </si>
+  <si>
+    <t>Consanguinity &amp; Funnel</t>
+  </si>
+  <si>
+    <t>https://marcneys.bandcamp.com/album/consanguinity-funnel</t>
+  </si>
+  <si>
+    <t>Naked Heart (Album)</t>
+  </si>
+  <si>
+    <t>https://jodyphilips.bandcamp.com/album/naked-heart-album</t>
+  </si>
+  <si>
+    <t>anonymous</t>
+  </si>
+  <si>
+    <t>https://autumna.bandcamp.com/album/anonymous</t>
+  </si>
+  <si>
+    <t>De Aanslag</t>
+  </si>
+  <si>
+    <t>https://wimnaudts.bandcamp.com/album/de-aanslag</t>
+  </si>
+  <si>
+    <t>Turtle Master &amp; Soul-T</t>
+  </si>
+  <si>
+    <t>Namur, Belgium</t>
+  </si>
+  <si>
+    <t>Let Me In (​+​Remixes)</t>
+  </si>
+  <si>
+    <t>https://turtmaster.bandcamp.com/album/let-me-in-remixes</t>
+  </si>
+  <si>
+    <t>Turtle Master</t>
+  </si>
+  <si>
+    <t>Yngvar</t>
+  </si>
+  <si>
+    <t>Tunes of Time</t>
+  </si>
+  <si>
+    <t>https://yngvar.bandcamp.com/album/tunes-of-time</t>
+  </si>
+  <si>
+    <t>DEAD x 文化</t>
+  </si>
+  <si>
+    <t>https://kontorasuto.bandcamp.com/album/dead-x</t>
+  </si>
+  <si>
+    <t>Soir Après Soir</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>https://soirapressoir.bandcamp.com/album/sas</t>
+  </si>
+  <si>
+    <t>Soundsource</t>
+  </si>
+  <si>
+    <t>Twin Brothers</t>
+  </si>
+  <si>
+    <t>https://soundsourceofficial.bandcamp.com/album/twin-brothers</t>
+  </si>
+  <si>
+    <t>Various Artists</t>
+  </si>
+  <si>
+    <t>Stilllysm</t>
+  </si>
+  <si>
+    <t>https://stilll.bandcamp.com/album/stilllysm</t>
+  </si>
+  <si>
+    <t>Café des Chansons</t>
+  </si>
+  <si>
+    <t>https://charlottehaesen.bandcamp.com/album/caf-des-chansons</t>
+  </si>
+  <si>
+    <t>CHARLOTTE HAESEN</t>
+  </si>
+  <si>
+    <t>Various Artists - Goa Madness Records</t>
+  </si>
+  <si>
+    <t>Phases Of Madness</t>
+  </si>
+  <si>
+    <t>https://goamadnessrecords.bandcamp.com/album/phases-of-madness</t>
+  </si>
+  <si>
+    <t>Arabesque Distribution</t>
+  </si>
+  <si>
+    <t>Still 23</t>
+  </si>
+  <si>
+    <t>Make Punk​-​Rock Great Again!</t>
+  </si>
+  <si>
+    <t>https://still23.bandcamp.com/album/make-punk-rock-great-again</t>
+  </si>
+  <si>
+    <t>OOSTERKOTS</t>
+  </si>
+  <si>
+    <t>Dikke Bocht</t>
+  </si>
+  <si>
+    <t>https://oosterkots.bandcamp.com/album/dikke-bocht</t>
+  </si>
+  <si>
+    <t>Aboubakar Traore &amp; Balima Foly</t>
+  </si>
+  <si>
+    <t>Wasso</t>
+  </si>
+  <si>
+    <t>https://balimafoly.bandcamp.com/album/wasso</t>
+  </si>
+  <si>
+    <t>The Psychedelic Underground Generation</t>
+  </si>
+  <si>
+    <t>Psychedelic Underground Generation # 36</t>
+  </si>
+  <si>
+    <t>https://pugrock.bandcamp.com/album/psychedelic-underground-generation-36</t>
+  </si>
+  <si>
+    <t>Kant Tery</t>
+  </si>
+  <si>
+    <t>First Stop</t>
+  </si>
+  <si>
+    <t>https://kanttery.bandcamp.com/album/first-stop</t>
+  </si>
+  <si>
+    <t>Nate Wooley</t>
+  </si>
+  <si>
+    <t>Le Roeulx, Belgium</t>
+  </si>
+  <si>
+    <t>Polychoral</t>
+  </si>
+  <si>
+    <t>https://mnoad.bandcamp.com/album/polychoral</t>
+  </si>
+  <si>
+    <t>MNÓAD</t>
+  </si>
+  <si>
+    <t>Digid</t>
+  </si>
+  <si>
+    <t>Gun Talk EP</t>
+  </si>
+  <si>
+    <t>https://halogenmusicgroup.bandcamp.com/album/gun-talk-ep</t>
+  </si>
+  <si>
+    <t>HalogenMusic</t>
+  </si>
+  <si>
+    <t>Halibab Matador</t>
+  </si>
+  <si>
+    <t>Braine L'Alleud, Belgium</t>
+  </si>
+  <si>
+    <t>Beats 3</t>
+  </si>
+  <si>
+    <t>https://albanmurenzi.bandcamp.com/album/beats-3-2</t>
+  </si>
+  <si>
+    <t>Khel</t>
+  </si>
+  <si>
+    <t>Sleepless</t>
+  </si>
+  <si>
+    <t>https://musicalexcrements.bandcamp.com/album/sleepless</t>
+  </si>
+  <si>
+    <t>Quanto // Polegar</t>
+  </si>
+  <si>
+    <t>https://luan--ecsu.bandcamp.com/album/quanto-polegar</t>
+  </si>
+  <si>
+    <t>Dempha // Terplin</t>
+  </si>
+  <si>
+    <t>https://luan--ecsu.bandcamp.com/album/dempha-terplin</t>
+  </si>
+  <si>
+    <t>A Perfect Friend</t>
+  </si>
+  <si>
+    <t>https://stilll.bandcamp.com/album/a-perfect-friend</t>
+  </si>
+  <si>
+    <t>Immune</t>
+  </si>
+  <si>
+    <t>The Sound Inside</t>
+  </si>
+  <si>
+    <t>https://stilll.bandcamp.com/album/the-sound-inside</t>
+  </si>
+  <si>
+    <t>Costa Music</t>
+  </si>
+  <si>
+    <t>Lighter Subjects</t>
+  </si>
+  <si>
+    <t>https://stilll.bandcamp.com/album/lighter-subjects</t>
+  </si>
+  <si>
+    <t>GLOED</t>
+  </si>
+  <si>
+    <t>https://gloed.bandcamp.com/album/gloed</t>
+  </si>
+  <si>
+    <t>Poppy Ruth Silver &amp; HS</t>
+  </si>
+  <si>
+    <t>FREEDOM IS SELECTIVE</t>
+  </si>
+  <si>
+    <t>https://hierarchysucks.bandcamp.com/album/freedom-is-selective</t>
+  </si>
+  <si>
+    <t>Nitr // Heatdriven</t>
+  </si>
+  <si>
+    <t>https://luan--ecsu.bandcamp.com/album/nitr-heatdriven</t>
+  </si>
+  <si>
+    <t>manducator</t>
+  </si>
+  <si>
+    <t>butterfly ep</t>
+  </si>
+  <si>
+    <t>https://manducator.bandcamp.com/album/butterfly-ep</t>
+  </si>
+  <si>
+    <t>The Bear Honk of the Reckless King</t>
+  </si>
+  <si>
+    <t>Summer Live</t>
+  </si>
+  <si>
+    <t>https://tbhotrk.bandcamp.com/album/summer-live</t>
+  </si>
+  <si>
+    <t>CHAOs ab</t>
+  </si>
+  <si>
+    <t>Close Encounter of Another Kind</t>
+  </si>
+  <si>
+    <t>https://chaosab.bandcamp.com/album/close-encounter-of-another-kind</t>
+  </si>
+  <si>
+    <t>Outerspace 2​.​5</t>
+  </si>
+  <si>
+    <t>https://neofujimuzik.bandcamp.com/album/outerspace-25</t>
+  </si>
+  <si>
+    <t>Mt.X (Natsu Fuji &amp; Jvst X)</t>
+  </si>
+  <si>
+    <t>Mt​.​X</t>
+  </si>
+  <si>
+    <t>https://neofujimuzik.bandcamp.com/album/mt-x</t>
+  </si>
+  <si>
+    <t>Ulgra</t>
+  </si>
+  <si>
+    <t>Pure Dickery</t>
+  </si>
+  <si>
+    <t>https://ulgra.bandcamp.com/album/pure-dickery</t>
+  </si>
+  <si>
+    <t>Hierarchy Sucks_PR0001</t>
+  </si>
+  <si>
+    <t>https://hierarchysucks.bandcamp.com/album/hierarchy-sucks-pr0001</t>
+  </si>
+  <si>
+    <t>ante-rasa</t>
+  </si>
+  <si>
+    <t>Liege, Belgium</t>
+  </si>
+  <si>
+    <t>ANTE05 - ∆☄O∆∆ - Sovetskaya</t>
+  </si>
+  <si>
+    <t>https://ante-rasa.bandcamp.com/album/ante05-o-sovetskaya</t>
+  </si>
+  <si>
+    <t>rリiチcャhーaドr_d</t>
+  </si>
+  <si>
+    <t>It's Only A Dream</t>
+  </si>
+  <si>
+    <t>https://richard04-08.bandcamp.com/album/its-only-a-dream</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1576,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1059,10 +1632,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3732,7 +4305,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>225</v>
       </c>
@@ -3752,8 +4325,2152 @@
         <v>227</v>
       </c>
     </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>322</v>
+      </c>
+      <c r="B114" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C114" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" t="s">
+        <v>323</v>
+      </c>
+      <c r="E114" t="s">
+        <v>324</v>
+      </c>
+      <c r="F114" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>326</v>
+      </c>
+      <c r="B115" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>108</v>
+      </c>
+      <c r="E115" t="s">
+        <v>327</v>
+      </c>
+      <c r="F115" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>326</v>
+      </c>
+      <c r="B116" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C116" t="s">
+        <v>62</v>
+      </c>
+      <c r="D116" t="s">
+        <v>108</v>
+      </c>
+      <c r="E116" t="s">
+        <v>327</v>
+      </c>
+      <c r="F116" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>329</v>
+      </c>
+      <c r="B117" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>63</v>
+      </c>
+      <c r="E117" t="s">
+        <v>330</v>
+      </c>
+      <c r="F117" t="s">
+        <v>331</v>
+      </c>
+      <c r="G117" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>329</v>
+      </c>
+      <c r="B118" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C118" t="s">
+        <v>62</v>
+      </c>
+      <c r="D118" t="s">
+        <v>63</v>
+      </c>
+      <c r="E118" t="s">
+        <v>330</v>
+      </c>
+      <c r="F118" t="s">
+        <v>331</v>
+      </c>
+      <c r="G118" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>332</v>
+      </c>
+      <c r="B119" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>21</v>
+      </c>
+      <c r="E119" t="s">
+        <v>333</v>
+      </c>
+      <c r="F119" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>335</v>
+      </c>
+      <c r="B120" s="3">
+        <v>42756</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" t="s">
+        <v>21</v>
+      </c>
+      <c r="E120" t="s">
+        <v>336</v>
+      </c>
+      <c r="F120" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>338</v>
+      </c>
+      <c r="B121" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>21</v>
+      </c>
+      <c r="E121" t="s">
+        <v>339</v>
+      </c>
+      <c r="F121" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>341</v>
+      </c>
+      <c r="B122" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" t="s">
+        <v>21</v>
+      </c>
+      <c r="E122" t="s">
+        <v>342</v>
+      </c>
+      <c r="F122" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>344</v>
+      </c>
+      <c r="B123" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" t="s">
+        <v>21</v>
+      </c>
+      <c r="E123" t="s">
+        <v>345</v>
+      </c>
+      <c r="F123" t="s">
+        <v>346</v>
+      </c>
+      <c r="G123" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>344</v>
+      </c>
+      <c r="B124" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C124" t="s">
+        <v>56</v>
+      </c>
+      <c r="D124" t="s">
+        <v>21</v>
+      </c>
+      <c r="E124" t="s">
+        <v>345</v>
+      </c>
+      <c r="F124" t="s">
+        <v>346</v>
+      </c>
+      <c r="G124" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>348</v>
+      </c>
+      <c r="B125" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" t="s">
+        <v>21</v>
+      </c>
+      <c r="E125" t="s">
+        <v>349</v>
+      </c>
+      <c r="F125" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>351</v>
+      </c>
+      <c r="B126" s="3">
+        <v>42750</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" t="s">
+        <v>21</v>
+      </c>
+      <c r="E126" t="s">
+        <v>352</v>
+      </c>
+      <c r="F126" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>354</v>
+      </c>
+      <c r="B127" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" t="s">
+        <v>21</v>
+      </c>
+      <c r="E127" t="s">
+        <v>355</v>
+      </c>
+      <c r="F127" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>357</v>
+      </c>
+      <c r="B128" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C128" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" t="s">
+        <v>21</v>
+      </c>
+      <c r="E128" t="s">
+        <v>358</v>
+      </c>
+      <c r="F128" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>360</v>
+      </c>
+      <c r="B129" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C129" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" t="s">
+        <v>21</v>
+      </c>
+      <c r="E129" t="s">
+        <v>361</v>
+      </c>
+      <c r="F129" t="s">
+        <v>362</v>
+      </c>
+      <c r="G129" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>364</v>
+      </c>
+      <c r="B130" s="3">
+        <v>42750</v>
+      </c>
+      <c r="C130" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" t="s">
+        <v>21</v>
+      </c>
+      <c r="E130" t="s">
+        <v>365</v>
+      </c>
+      <c r="F130" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>367</v>
+      </c>
+      <c r="B131" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C131" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" t="s">
+        <v>26</v>
+      </c>
+      <c r="E131" t="s">
+        <v>368</v>
+      </c>
+      <c r="F131" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>370</v>
+      </c>
+      <c r="B132" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C132" t="s">
+        <v>8</v>
+      </c>
+      <c r="D132" t="s">
+        <v>26</v>
+      </c>
+      <c r="E132" t="s">
+        <v>371</v>
+      </c>
+      <c r="F132" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>370</v>
+      </c>
+      <c r="B133" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C133" t="s">
+        <v>62</v>
+      </c>
+      <c r="D133" t="s">
+        <v>26</v>
+      </c>
+      <c r="E133" t="s">
+        <v>371</v>
+      </c>
+      <c r="F133" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>373</v>
+      </c>
+      <c r="B134" s="3">
+        <v>42759</v>
+      </c>
+      <c r="C134" t="s">
+        <v>8</v>
+      </c>
+      <c r="D134" t="s">
+        <v>26</v>
+      </c>
+      <c r="E134" t="s">
+        <v>374</v>
+      </c>
+      <c r="F134" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>373</v>
+      </c>
+      <c r="B135" s="3">
+        <v>42759</v>
+      </c>
+      <c r="C135" t="s">
+        <v>104</v>
+      </c>
+      <c r="D135" t="s">
+        <v>26</v>
+      </c>
+      <c r="E135" t="s">
+        <v>374</v>
+      </c>
+      <c r="F135" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>376</v>
+      </c>
+      <c r="B136" s="3">
+        <v>42758</v>
+      </c>
+      <c r="C136" t="s">
+        <v>8</v>
+      </c>
+      <c r="D136" t="s">
+        <v>26</v>
+      </c>
+      <c r="E136" t="s">
+        <v>377</v>
+      </c>
+      <c r="F136" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>379</v>
+      </c>
+      <c r="B137" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C137" t="s">
+        <v>8</v>
+      </c>
+      <c r="D137" t="s">
+        <v>26</v>
+      </c>
+      <c r="E137" t="s">
+        <v>380</v>
+      </c>
+      <c r="F137" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>382</v>
+      </c>
+      <c r="B138" s="3">
+        <v>42766</v>
+      </c>
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" t="s">
+        <v>26</v>
+      </c>
+      <c r="E138" t="s">
+        <v>383</v>
+      </c>
+      <c r="F138" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>387</v>
+      </c>
+      <c r="B139" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C139" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" t="s">
+        <v>388</v>
+      </c>
+      <c r="E139" t="s">
+        <v>389</v>
+      </c>
+      <c r="F139" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>391</v>
+      </c>
+      <c r="B140" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C140" t="s">
+        <v>104</v>
+      </c>
+      <c r="D140" t="s">
+        <v>392</v>
+      </c>
+      <c r="E140" t="s">
+        <v>393</v>
+      </c>
+      <c r="F140" t="s">
+        <v>394</v>
+      </c>
+      <c r="G140" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>396</v>
+      </c>
+      <c r="B141" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C141" t="s">
+        <v>8</v>
+      </c>
+      <c r="D141" t="s">
+        <v>392</v>
+      </c>
+      <c r="E141" t="s">
+        <v>397</v>
+      </c>
+      <c r="F141" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>399</v>
+      </c>
+      <c r="B142" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" t="s">
+        <v>400</v>
+      </c>
+      <c r="E142" t="s">
+        <v>401</v>
+      </c>
+      <c r="F142" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>30</v>
+      </c>
+      <c r="B143" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" t="s">
+        <v>31</v>
+      </c>
+      <c r="E143" t="s">
+        <v>403</v>
+      </c>
+      <c r="F143" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>12</v>
+      </c>
+      <c r="B144" s="3">
+        <v>42736</v>
+      </c>
+      <c r="C144" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
+        <v>13</v>
+      </c>
+      <c r="E144" t="s">
+        <v>405</v>
+      </c>
+      <c r="F144" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>318</v>
+      </c>
+      <c r="B145" s="3">
+        <v>42762</v>
+      </c>
+      <c r="C145" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" t="s">
+        <v>319</v>
+      </c>
+      <c r="E145" t="s">
+        <v>407</v>
+      </c>
+      <c r="F145" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>385</v>
+      </c>
+      <c r="B146" s="3">
+        <v>42762</v>
+      </c>
+      <c r="C146" t="s">
+        <v>8</v>
+      </c>
+      <c r="D146" t="s">
+        <v>386</v>
+      </c>
+      <c r="E146" t="s">
+        <v>409</v>
+      </c>
+      <c r="F146" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>411</v>
+      </c>
+      <c r="B147" s="3">
+        <v>42762</v>
+      </c>
+      <c r="C147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147" t="s">
+        <v>412</v>
+      </c>
+      <c r="E147" t="s">
+        <v>413</v>
+      </c>
+      <c r="F147" t="s">
+        <v>414</v>
+      </c>
+      <c r="G147" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>416</v>
+      </c>
+      <c r="B148" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C148" t="s">
+        <v>8</v>
+      </c>
+      <c r="D148" t="s">
+        <v>9</v>
+      </c>
+      <c r="E148" t="s">
+        <v>417</v>
+      </c>
+      <c r="F148" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>367</v>
+      </c>
+      <c r="B149" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C149" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149" t="s">
+        <v>26</v>
+      </c>
+      <c r="E149" t="s">
+        <v>368</v>
+      </c>
+      <c r="F149" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>322</v>
+      </c>
+      <c r="B150" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C150" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150" t="s">
+        <v>323</v>
+      </c>
+      <c r="E150" t="s">
+        <v>324</v>
+      </c>
+      <c r="F150" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>231</v>
+      </c>
+      <c r="B151" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C151" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" t="s">
+        <v>9</v>
+      </c>
+      <c r="E151" t="s">
+        <v>419</v>
+      </c>
+      <c r="F151" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>421</v>
+      </c>
+      <c r="B152" s="3">
+        <v>42761</v>
+      </c>
+      <c r="C152" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" t="s">
+        <v>241</v>
+      </c>
+      <c r="E152" t="s">
+        <v>422</v>
+      </c>
+      <c r="F152" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>424</v>
+      </c>
+      <c r="B153" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C153" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153" t="s">
+        <v>425</v>
+      </c>
+      <c r="F153" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>427</v>
+      </c>
+      <c r="B154" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C154" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" t="s">
+        <v>9</v>
+      </c>
+      <c r="E154" t="s">
+        <v>428</v>
+      </c>
+      <c r="F154" t="s">
+        <v>429</v>
+      </c>
+      <c r="G154" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>427</v>
+      </c>
+      <c r="B155" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C155" t="s">
+        <v>62</v>
+      </c>
+      <c r="D155" t="s">
+        <v>9</v>
+      </c>
+      <c r="E155" t="s">
+        <v>428</v>
+      </c>
+      <c r="F155" t="s">
+        <v>429</v>
+      </c>
+      <c r="G155" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>370</v>
+      </c>
+      <c r="B156" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C156" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" t="s">
+        <v>26</v>
+      </c>
+      <c r="E156" t="s">
+        <v>371</v>
+      </c>
+      <c r="F156" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>370</v>
+      </c>
+      <c r="B157" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C157" t="s">
+        <v>62</v>
+      </c>
+      <c r="D157" t="s">
+        <v>26</v>
+      </c>
+      <c r="E157" t="s">
+        <v>371</v>
+      </c>
+      <c r="F157" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>430</v>
+      </c>
+      <c r="B158" s="3">
+        <v>42765</v>
+      </c>
+      <c r="C158" t="s">
+        <v>8</v>
+      </c>
+      <c r="D158" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158" t="s">
+        <v>430</v>
+      </c>
+      <c r="F158" t="s">
+        <v>431</v>
+      </c>
+      <c r="G158" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>373</v>
+      </c>
+      <c r="B159" s="3">
+        <v>42759</v>
+      </c>
+      <c r="C159" t="s">
+        <v>8</v>
+      </c>
+      <c r="D159" t="s">
+        <v>26</v>
+      </c>
+      <c r="E159" t="s">
+        <v>374</v>
+      </c>
+      <c r="F159" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>373</v>
+      </c>
+      <c r="B160" s="3">
+        <v>42759</v>
+      </c>
+      <c r="C160" t="s">
+        <v>104</v>
+      </c>
+      <c r="D160" t="s">
+        <v>26</v>
+      </c>
+      <c r="E160" t="s">
+        <v>374</v>
+      </c>
+      <c r="F160" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>433</v>
+      </c>
+      <c r="B161" s="3">
+        <v>42762</v>
+      </c>
+      <c r="C161" t="s">
+        <v>62</v>
+      </c>
+      <c r="D161" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161" t="s">
+        <v>434</v>
+      </c>
+      <c r="F161" t="s">
+        <v>435</v>
+      </c>
+      <c r="G161" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>433</v>
+      </c>
+      <c r="B162" s="3">
+        <v>42762</v>
+      </c>
+      <c r="C162" t="s">
+        <v>8</v>
+      </c>
+      <c r="D162" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162" t="s">
+        <v>434</v>
+      </c>
+      <c r="F162" t="s">
+        <v>435</v>
+      </c>
+      <c r="G162" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>387</v>
+      </c>
+      <c r="B163" s="3">
+        <v>42760</v>
+      </c>
+      <c r="C163" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" t="s">
+        <v>388</v>
+      </c>
+      <c r="E163" t="s">
+        <v>389</v>
+      </c>
+      <c r="F163" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C164" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" t="s">
+        <v>108</v>
+      </c>
+      <c r="E164" t="s">
+        <v>327</v>
+      </c>
+      <c r="F164" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>326</v>
+      </c>
+      <c r="B165" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C165" t="s">
+        <v>62</v>
+      </c>
+      <c r="D165" t="s">
+        <v>108</v>
+      </c>
+      <c r="E165" t="s">
+        <v>327</v>
+      </c>
+      <c r="F165" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>437</v>
+      </c>
+      <c r="B166" s="3">
+        <v>42759</v>
+      </c>
+      <c r="C166" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166" t="s">
+        <v>438</v>
+      </c>
+      <c r="F166" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>440</v>
+      </c>
+      <c r="B167" s="3">
+        <v>42759</v>
+      </c>
+      <c r="C167" t="s">
+        <v>8</v>
+      </c>
+      <c r="D167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167" t="s">
+        <v>441</v>
+      </c>
+      <c r="F167" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>332</v>
+      </c>
+      <c r="B168" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C168" t="s">
+        <v>8</v>
+      </c>
+      <c r="D168" t="s">
+        <v>21</v>
+      </c>
+      <c r="E168" t="s">
+        <v>333</v>
+      </c>
+      <c r="F168" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>335</v>
+      </c>
+      <c r="B169" s="3">
+        <v>42756</v>
+      </c>
+      <c r="C169" t="s">
+        <v>8</v>
+      </c>
+      <c r="D169" t="s">
+        <v>21</v>
+      </c>
+      <c r="E169" t="s">
+        <v>336</v>
+      </c>
+      <c r="F169" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C170" t="s">
+        <v>8</v>
+      </c>
+      <c r="D170" t="s">
+        <v>21</v>
+      </c>
+      <c r="E170" t="s">
+        <v>339</v>
+      </c>
+      <c r="F170" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>443</v>
+      </c>
+      <c r="B171" s="3">
+        <v>42758</v>
+      </c>
+      <c r="C171" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171" t="s">
+        <v>444</v>
+      </c>
+      <c r="F171" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>376</v>
+      </c>
+      <c r="B172" s="3">
+        <v>42758</v>
+      </c>
+      <c r="C172" t="s">
+        <v>8</v>
+      </c>
+      <c r="D172" t="s">
+        <v>26</v>
+      </c>
+      <c r="E172" t="s">
+        <v>377</v>
+      </c>
+      <c r="F172" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>446</v>
+      </c>
+      <c r="B173" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C173" t="s">
+        <v>8</v>
+      </c>
+      <c r="D173" t="s">
+        <v>9</v>
+      </c>
+      <c r="E173" t="s">
+        <v>447</v>
+      </c>
+      <c r="F173" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>449</v>
+      </c>
+      <c r="B174" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C174" t="s">
+        <v>8</v>
+      </c>
+      <c r="D174" t="s">
+        <v>9</v>
+      </c>
+      <c r="E174" t="s">
+        <v>450</v>
+      </c>
+      <c r="F174" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>452</v>
+      </c>
+      <c r="B175" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C175" t="s">
+        <v>8</v>
+      </c>
+      <c r="D175" t="s">
+        <v>453</v>
+      </c>
+      <c r="E175" t="s">
+        <v>454</v>
+      </c>
+      <c r="F175" t="s">
+        <v>455</v>
+      </c>
+      <c r="G175" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>452</v>
+      </c>
+      <c r="B176" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C176" t="s">
+        <v>62</v>
+      </c>
+      <c r="D176" t="s">
+        <v>453</v>
+      </c>
+      <c r="E176" t="s">
+        <v>454</v>
+      </c>
+      <c r="F176" t="s">
+        <v>455</v>
+      </c>
+      <c r="G176" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>399</v>
+      </c>
+      <c r="B177" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C177" t="s">
+        <v>8</v>
+      </c>
+      <c r="D177" t="s">
+        <v>400</v>
+      </c>
+      <c r="E177" t="s">
+        <v>401</v>
+      </c>
+      <c r="F177" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>457</v>
+      </c>
+      <c r="B178" s="3">
+        <v>42758</v>
+      </c>
+      <c r="C178" t="s">
+        <v>8</v>
+      </c>
+      <c r="D178" t="s">
+        <v>9</v>
+      </c>
+      <c r="E178" t="s">
+        <v>458</v>
+      </c>
+      <c r="F178" t="s">
+        <v>459</v>
+      </c>
+      <c r="G178" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>461</v>
+      </c>
+      <c r="B179" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C179" t="s">
+        <v>8</v>
+      </c>
+      <c r="D179" t="s">
+        <v>462</v>
+      </c>
+      <c r="E179" t="s">
+        <v>463</v>
+      </c>
+      <c r="F179" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>341</v>
+      </c>
+      <c r="B180" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C180" t="s">
+        <v>8</v>
+      </c>
+      <c r="D180" t="s">
+        <v>21</v>
+      </c>
+      <c r="E180" t="s">
+        <v>342</v>
+      </c>
+      <c r="F180" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>465</v>
+      </c>
+      <c r="B181" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C181" t="s">
+        <v>8</v>
+      </c>
+      <c r="D181" t="s">
+        <v>9</v>
+      </c>
+      <c r="E181" t="s">
+        <v>466</v>
+      </c>
+      <c r="F181" t="s">
+        <v>467</v>
+      </c>
+      <c r="G181" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>69</v>
+      </c>
+      <c r="B182" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C182" t="s">
+        <v>8</v>
+      </c>
+      <c r="D182" t="s">
+        <v>9</v>
+      </c>
+      <c r="E182" t="s">
+        <v>468</v>
+      </c>
+      <c r="F182" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>69</v>
+      </c>
+      <c r="B183" s="3">
+        <v>42757</v>
+      </c>
+      <c r="C183" t="s">
+        <v>8</v>
+      </c>
+      <c r="D183" t="s">
+        <v>9</v>
+      </c>
+      <c r="E183" t="s">
+        <v>470</v>
+      </c>
+      <c r="F183" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>265</v>
+      </c>
+      <c r="B184" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C184" t="s">
+        <v>8</v>
+      </c>
+      <c r="D184" t="s">
+        <v>9</v>
+      </c>
+      <c r="E184" t="s">
+        <v>472</v>
+      </c>
+      <c r="F184" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>265</v>
+      </c>
+      <c r="B185" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C185" t="s">
+        <v>62</v>
+      </c>
+      <c r="D185" t="s">
+        <v>9</v>
+      </c>
+      <c r="E185" t="s">
+        <v>472</v>
+      </c>
+      <c r="F185" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>474</v>
+      </c>
+      <c r="B186" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C186" t="s">
+        <v>8</v>
+      </c>
+      <c r="D186" t="s">
+        <v>9</v>
+      </c>
+      <c r="E186" t="s">
+        <v>475</v>
+      </c>
+      <c r="F186" t="s">
+        <v>476</v>
+      </c>
+      <c r="G186" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>474</v>
+      </c>
+      <c r="B187" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C187" t="s">
+        <v>62</v>
+      </c>
+      <c r="D187" t="s">
+        <v>9</v>
+      </c>
+      <c r="E187" t="s">
+        <v>475</v>
+      </c>
+      <c r="F187" t="s">
+        <v>476</v>
+      </c>
+      <c r="G187" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>477</v>
+      </c>
+      <c r="B188" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C188" t="s">
+        <v>8</v>
+      </c>
+      <c r="D188" t="s">
+        <v>9</v>
+      </c>
+      <c r="E188" t="s">
+        <v>478</v>
+      </c>
+      <c r="F188" t="s">
+        <v>479</v>
+      </c>
+      <c r="G188" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>477</v>
+      </c>
+      <c r="B189" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C189" t="s">
+        <v>62</v>
+      </c>
+      <c r="D189" t="s">
+        <v>9</v>
+      </c>
+      <c r="E189" t="s">
+        <v>478</v>
+      </c>
+      <c r="F189" t="s">
+        <v>479</v>
+      </c>
+      <c r="G189" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>480</v>
+      </c>
+      <c r="B190" s="3">
+        <v>42756</v>
+      </c>
+      <c r="C190" t="s">
+        <v>8</v>
+      </c>
+      <c r="D190" t="s">
+        <v>9</v>
+      </c>
+      <c r="E190" t="s">
+        <v>480</v>
+      </c>
+      <c r="F190" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>482</v>
+      </c>
+      <c r="B191" s="3">
+        <v>42756</v>
+      </c>
+      <c r="C191" t="s">
+        <v>8</v>
+      </c>
+      <c r="D191" t="s">
+        <v>9</v>
+      </c>
+      <c r="E191" t="s">
+        <v>483</v>
+      </c>
+      <c r="F191" t="s">
+        <v>484</v>
+      </c>
+      <c r="G191" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>69</v>
+      </c>
+      <c r="B192" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C192" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" t="s">
+        <v>9</v>
+      </c>
+      <c r="E192" t="s">
+        <v>485</v>
+      </c>
+      <c r="F192" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>391</v>
+      </c>
+      <c r="B193" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C193" t="s">
+        <v>104</v>
+      </c>
+      <c r="D193" t="s">
+        <v>392</v>
+      </c>
+      <c r="E193" t="s">
+        <v>393</v>
+      </c>
+      <c r="F193" t="s">
+        <v>394</v>
+      </c>
+      <c r="G193" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>487</v>
+      </c>
+      <c r="B194" s="3">
+        <v>42755</v>
+      </c>
+      <c r="C194" t="s">
+        <v>8</v>
+      </c>
+      <c r="D194" t="s">
+        <v>9</v>
+      </c>
+      <c r="E194" t="s">
+        <v>488</v>
+      </c>
+      <c r="F194" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>379</v>
+      </c>
+      <c r="B195" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C195" t="s">
+        <v>8</v>
+      </c>
+      <c r="D195" t="s">
+        <v>26</v>
+      </c>
+      <c r="E195" t="s">
+        <v>380</v>
+      </c>
+      <c r="F195" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>490</v>
+      </c>
+      <c r="B196" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C196" t="s">
+        <v>8</v>
+      </c>
+      <c r="D196" t="s">
+        <v>42</v>
+      </c>
+      <c r="E196" t="s">
+        <v>491</v>
+      </c>
+      <c r="F196" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>344</v>
+      </c>
+      <c r="B197" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C197" t="s">
+        <v>8</v>
+      </c>
+      <c r="D197" t="s">
+        <v>21</v>
+      </c>
+      <c r="E197" t="s">
+        <v>345</v>
+      </c>
+      <c r="F197" t="s">
+        <v>346</v>
+      </c>
+      <c r="G197" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>344</v>
+      </c>
+      <c r="B198" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C198" t="s">
+        <v>56</v>
+      </c>
+      <c r="D198" t="s">
+        <v>21</v>
+      </c>
+      <c r="E198" t="s">
+        <v>345</v>
+      </c>
+      <c r="F198" t="s">
+        <v>346</v>
+      </c>
+      <c r="G198" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>493</v>
+      </c>
+      <c r="B199" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C199" t="s">
+        <v>8</v>
+      </c>
+      <c r="D199" t="s">
+        <v>9</v>
+      </c>
+      <c r="E199" t="s">
+        <v>494</v>
+      </c>
+      <c r="F199" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>315</v>
+      </c>
+      <c r="B200" s="3">
+        <v>42754</v>
+      </c>
+      <c r="C200" t="s">
+        <v>8</v>
+      </c>
+      <c r="D200" t="s">
+        <v>9</v>
+      </c>
+      <c r="E200" t="s">
+        <v>496</v>
+      </c>
+      <c r="F200" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>348</v>
+      </c>
+      <c r="B201" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C201" t="s">
+        <v>8</v>
+      </c>
+      <c r="D201" t="s">
+        <v>21</v>
+      </c>
+      <c r="E201" t="s">
+        <v>349</v>
+      </c>
+      <c r="F201" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>498</v>
+      </c>
+      <c r="B202" s="3">
+        <v>42750</v>
+      </c>
+      <c r="C202" t="s">
+        <v>8</v>
+      </c>
+      <c r="D202" t="s">
+        <v>9</v>
+      </c>
+      <c r="E202" t="s">
+        <v>499</v>
+      </c>
+      <c r="F202" t="s">
+        <v>500</v>
+      </c>
+      <c r="G202" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>351</v>
+      </c>
+      <c r="B203" s="3">
+        <v>42750</v>
+      </c>
+      <c r="C203" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" t="s">
+        <v>21</v>
+      </c>
+      <c r="E203" t="s">
+        <v>352</v>
+      </c>
+      <c r="F203" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>396</v>
+      </c>
+      <c r="B204" s="3">
+        <v>42753</v>
+      </c>
+      <c r="C204" t="s">
+        <v>8</v>
+      </c>
+      <c r="D204" t="s">
+        <v>392</v>
+      </c>
+      <c r="E204" t="s">
+        <v>397</v>
+      </c>
+      <c r="F204" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>501</v>
+      </c>
+      <c r="B205" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C205" t="s">
+        <v>8</v>
+      </c>
+      <c r="D205" t="s">
+        <v>9</v>
+      </c>
+      <c r="E205" t="s">
+        <v>502</v>
+      </c>
+      <c r="F205" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>354</v>
+      </c>
+      <c r="B206" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C206" t="s">
+        <v>8</v>
+      </c>
+      <c r="D206" t="s">
+        <v>21</v>
+      </c>
+      <c r="E206" t="s">
+        <v>355</v>
+      </c>
+      <c r="F206" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>160</v>
+      </c>
+      <c r="B207" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C207" t="s">
+        <v>8</v>
+      </c>
+      <c r="D207" t="s">
+        <v>9</v>
+      </c>
+      <c r="E207" t="s">
+        <v>504</v>
+      </c>
+      <c r="F207" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>357</v>
+      </c>
+      <c r="B208" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C208" t="s">
+        <v>8</v>
+      </c>
+      <c r="D208" t="s">
+        <v>21</v>
+      </c>
+      <c r="E208" t="s">
+        <v>358</v>
+      </c>
+      <c r="F208" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>360</v>
+      </c>
+      <c r="B209" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C209" t="s">
+        <v>8</v>
+      </c>
+      <c r="D209" t="s">
+        <v>21</v>
+      </c>
+      <c r="E209" t="s">
+        <v>361</v>
+      </c>
+      <c r="F209" t="s">
+        <v>362</v>
+      </c>
+      <c r="G209" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>382</v>
+      </c>
+      <c r="B210" s="3">
+        <v>42766</v>
+      </c>
+      <c r="C210" t="s">
+        <v>8</v>
+      </c>
+      <c r="D210" t="s">
+        <v>26</v>
+      </c>
+      <c r="E210" t="s">
+        <v>383</v>
+      </c>
+      <c r="F210" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>329</v>
+      </c>
+      <c r="B211" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C211" t="s">
+        <v>8</v>
+      </c>
+      <c r="D211" t="s">
+        <v>63</v>
+      </c>
+      <c r="E211" t="s">
+        <v>330</v>
+      </c>
+      <c r="F211" t="s">
+        <v>331</v>
+      </c>
+      <c r="G211" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>329</v>
+      </c>
+      <c r="B212" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C212" t="s">
+        <v>62</v>
+      </c>
+      <c r="D212" t="s">
+        <v>63</v>
+      </c>
+      <c r="E212" t="s">
+        <v>330</v>
+      </c>
+      <c r="F212" t="s">
+        <v>331</v>
+      </c>
+      <c r="G212" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>506</v>
+      </c>
+      <c r="B213" s="3">
+        <v>42751</v>
+      </c>
+      <c r="C213" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" t="s">
+        <v>507</v>
+      </c>
+      <c r="E213" t="s">
+        <v>508</v>
+      </c>
+      <c r="F213" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>510</v>
+      </c>
+      <c r="B214" s="3">
+        <v>42750</v>
+      </c>
+      <c r="C214" t="s">
+        <v>8</v>
+      </c>
+      <c r="D214" t="s">
+        <v>9</v>
+      </c>
+      <c r="E214" t="s">
+        <v>511</v>
+      </c>
+      <c r="F214" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>364</v>
+      </c>
+      <c r="B215" s="3">
+        <v>42750</v>
+      </c>
+      <c r="C215" t="s">
+        <v>8</v>
+      </c>
+      <c r="D215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E215" t="s">
+        <v>365</v>
+      </c>
+      <c r="F215" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>12</v>
+      </c>
+      <c r="B216" s="3">
+        <v>42736</v>
+      </c>
+      <c r="C216" t="s">
+        <v>8</v>
+      </c>
+      <c r="D216" t="s">
+        <v>13</v>
+      </c>
+      <c r="E216" t="s">
+        <v>405</v>
+      </c>
+      <c r="F216" t="s">
+        <v>406</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H1">
+  <autoFilter ref="A1:H216">
     <sortState ref="A2:H113">
       <sortCondition ref="B1:B113"/>
     </sortState>

</xml_diff>

<commit_message>
commit van fixed (removed duplicates) dataset
</commit_message>
<xml_diff>
--- a/bandcamp_januari_01-02-2017.xlsx
+++ b/bandcamp_januari_01-02-2017.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="513">
   <si>
     <t>artist</t>
   </si>
@@ -1576,7 +1576,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1632,10 +1632,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1915,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A1:G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2316,30 +2316,27 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>42737</v>
+        <v>42736</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>198</v>
+        <v>405</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
-      </c>
-      <c r="G19" t="s">
-        <v>200</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B20" s="3">
         <v>42737</v>
@@ -2348,18 +2345,21 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F20" t="s">
-        <v>204</v>
+        <v>199</v>
+      </c>
+      <c r="G20" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B21" s="3">
         <v>42737</v>
@@ -2368,16 +2368,13 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="E21" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F21" t="s">
-        <v>206</v>
-      </c>
-      <c r="G21" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2388,7 +2385,7 @@
         <v>42737</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2405,27 +2402,30 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B23" s="3">
         <v>42737</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F23" t="s">
-        <v>209</v>
+        <v>206</v>
+      </c>
+      <c r="G23" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B24" s="3">
         <v>42737</v>
@@ -2434,24 +2434,21 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="F24" t="s">
-        <v>210</v>
-      </c>
-      <c r="G24" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="B25" s="3">
-        <v>42738</v>
+        <v>42737</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -2460,10 +2457,13 @@
         <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="F25" t="s">
-        <v>230</v>
+        <v>210</v>
+      </c>
+      <c r="G25" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2474,7 +2474,7 @@
         <v>42738</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
@@ -2488,27 +2488,27 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B27" s="3">
         <v>42738</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F27" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B28" s="3">
         <v>42738</v>
@@ -2520,15 +2520,15 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B29" s="3">
         <v>42738</v>
@@ -2537,18 +2537,18 @@
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F29" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B30" s="3">
         <v>42738</v>
@@ -2557,38 +2557,38 @@
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>241</v>
+        <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F30" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="B31" s="3">
-        <v>42739</v>
+        <v>42738</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>241</v>
       </c>
       <c r="E31" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F31" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B32" s="3">
         <v>42739</v>
@@ -2600,18 +2600,18 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F32" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B33" s="3">
-        <v>42741</v>
+        <v>42739</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -2620,15 +2620,15 @@
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F33" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B34" s="3">
         <v>42741</v>
@@ -2637,18 +2637,18 @@
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>253</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F34" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B35" s="3">
         <v>42741</v>
@@ -2657,18 +2657,18 @@
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="E35" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F35" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B36" s="3">
         <v>42741</v>
@@ -2677,18 +2677,18 @@
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>241</v>
       </c>
       <c r="E36" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F36" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B37" s="3">
         <v>42741</v>
@@ -2697,41 +2697,41 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F37" t="s">
-        <v>264</v>
-      </c>
-      <c r="G37" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B38" s="3">
-        <v>42742</v>
+        <v>42741</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>267</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F38" t="s">
-        <v>269</v>
+        <v>264</v>
+      </c>
+      <c r="G38" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B39" s="3">
         <v>42742</v>
@@ -2740,18 +2740,18 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>267</v>
       </c>
       <c r="E39" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F39" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B40" s="3">
         <v>42742</v>
@@ -2760,33 +2760,33 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F40" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B41" s="3">
         <v>42742</v>
       </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F41" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2797,7 +2797,7 @@
         <v>42742</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
         <v>108</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B43" s="3">
         <v>42742</v>
@@ -2820,38 +2820,38 @@
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="E43" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F43" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B44" s="3">
-        <v>42743</v>
+        <v>42742</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F44" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B45" s="3">
         <v>42743</v>
@@ -2860,21 +2860,18 @@
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F45" t="s">
-        <v>287</v>
-      </c>
-      <c r="G45" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B46" s="3">
         <v>42743</v>
@@ -2883,38 +2880,41 @@
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>290</v>
+        <v>35</v>
       </c>
       <c r="E46" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F46" t="s">
-        <v>292</v>
+        <v>287</v>
+      </c>
+      <c r="G46" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B47" s="3">
-        <v>42744</v>
+        <v>42743</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>290</v>
       </c>
       <c r="E47" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F47" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B48" s="3">
         <v>42744</v>
@@ -2926,18 +2926,15 @@
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F48" t="s">
-        <v>298</v>
-      </c>
-      <c r="G48" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B49" s="3">
         <v>42744</v>
@@ -2946,18 +2943,21 @@
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F49" t="s">
-        <v>302</v>
+        <v>298</v>
+      </c>
+      <c r="G49" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B50" s="3">
         <v>42744</v>
@@ -2966,61 +2966,61 @@
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E50" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F50" t="s">
-        <v>305</v>
-      </c>
-      <c r="G50" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B51" s="3">
         <v>42744</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F51" t="s">
-        <v>309</v>
+        <v>305</v>
+      </c>
+      <c r="G51" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B52" s="3">
         <v>42744</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F52" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>231</v>
+        <v>310</v>
       </c>
       <c r="B53" s="3">
         <v>42744</v>
@@ -3032,15 +3032,15 @@
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>315</v>
+        <v>231</v>
       </c>
       <c r="B54" s="3">
         <v>42744</v>
@@ -3052,15 +3052,15 @@
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F54" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B55" s="3">
         <v>42744</v>
@@ -3069,38 +3069,38 @@
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>319</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F55" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>318</v>
       </c>
       <c r="B56" s="3">
-        <v>42745</v>
+        <v>42744</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
       <c r="E56" t="s">
-        <v>70</v>
+        <v>320</v>
       </c>
       <c r="F56" t="s">
-        <v>71</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B57" s="3">
         <v>42745</v>
@@ -3112,15 +3112,15 @@
         <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F57" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B58" s="3">
         <v>42745</v>
@@ -3132,15 +3132,15 @@
         <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3">
         <v>42745</v>
@@ -3149,18 +3149,18 @@
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B60" s="3">
         <v>42745</v>
@@ -3169,18 +3169,18 @@
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B61" s="3">
         <v>42745</v>
@@ -3189,18 +3189,18 @@
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E61" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F61" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B62" s="3">
         <v>42745</v>
@@ -3209,18 +3209,18 @@
         <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F62" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B63" s="3">
         <v>42745</v>
@@ -3232,13 +3232,10 @@
         <v>21</v>
       </c>
       <c r="E63" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F63" t="s">
-        <v>91</v>
-      </c>
-      <c r="G63" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -3249,7 +3246,7 @@
         <v>42745</v>
       </c>
       <c r="C64" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D64" t="s">
         <v>21</v>
@@ -3266,25 +3263,25 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B65" s="3">
         <v>42745</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D65" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E65" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G65" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -3295,7 +3292,7 @@
         <v>42745</v>
       </c>
       <c r="C66" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
         <v>26</v>
@@ -3312,27 +3309,30 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B67" s="3">
-        <v>42746</v>
+        <v>42745</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D67" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="E67" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F67" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="G67" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B68" s="3">
         <v>42746</v>
@@ -3341,13 +3341,13 @@
         <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="E68" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F68" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -3358,7 +3358,7 @@
         <v>42746</v>
       </c>
       <c r="C69" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
         <v>21</v>
@@ -3372,27 +3372,27 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="B70" s="3">
         <v>42746</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E70" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F70" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="B71" s="3">
         <v>42746</v>
@@ -3401,21 +3401,18 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F71" t="s">
-        <v>110</v>
-      </c>
-      <c r="G71" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="B72" s="3">
         <v>42746</v>
@@ -3424,13 +3421,16 @@
         <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="E72" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F72" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="G72" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3438,7 +3438,7 @@
         <v>69</v>
       </c>
       <c r="B73" s="3">
-        <v>42747</v>
+        <v>42746</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -3447,18 +3447,18 @@
         <v>9</v>
       </c>
       <c r="E73" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="B74" s="3">
-        <v>42748</v>
+        <v>42747</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
@@ -3467,15 +3467,15 @@
         <v>9</v>
       </c>
       <c r="E74" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F74" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B75" s="3">
         <v>42748</v>
@@ -3484,21 +3484,18 @@
         <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E75" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F75" t="s">
-        <v>121</v>
-      </c>
-      <c r="G75" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B76" s="3">
         <v>42748</v>
@@ -3507,18 +3504,21 @@
         <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="E76" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F76" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="G76" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B77" s="3">
         <v>42748</v>
@@ -3527,16 +3527,13 @@
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F77" t="s">
-        <v>127</v>
-      </c>
-      <c r="G77" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -3547,7 +3544,7 @@
         <v>42748</v>
       </c>
       <c r="C78" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D78" t="s">
         <v>26</v>
@@ -3564,27 +3561,30 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B79" s="3">
         <v>42748</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D79" t="s">
         <v>26</v>
       </c>
       <c r="E79" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F79" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="G79" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B80" s="3">
         <v>42748</v>
@@ -3593,21 +3593,18 @@
         <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>132</v>
+        <v>26</v>
       </c>
       <c r="E80" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F80" t="s">
-        <v>134</v>
-      </c>
-      <c r="G80" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B81" s="3">
         <v>42748</v>
@@ -3616,21 +3613,21 @@
         <v>8</v>
       </c>
       <c r="D81" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="E81" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F81" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G81" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B82" s="3">
         <v>42748</v>
@@ -3639,18 +3636,21 @@
         <v>8</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F82" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="G82" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="B83" s="3">
         <v>42748</v>
@@ -3662,15 +3662,15 @@
         <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F83" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="B84" s="3">
         <v>42748</v>
@@ -3679,16 +3679,13 @@
         <v>8</v>
       </c>
       <c r="D84" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F84" t="s">
-        <v>146</v>
-      </c>
-      <c r="G84" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -3699,7 +3696,7 @@
         <v>42748</v>
       </c>
       <c r="C85" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D85" t="s">
         <v>132</v>
@@ -3722,7 +3719,7 @@
         <v>42748</v>
       </c>
       <c r="C86" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="D86" t="s">
         <v>132</v>
@@ -3739,30 +3736,30 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B87" s="3">
-        <v>42749</v>
+        <v>42748</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>132</v>
       </c>
       <c r="E87" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F87" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G87" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B88" s="3">
         <v>42749</v>
@@ -3771,16 +3768,16 @@
         <v>8</v>
       </c>
       <c r="D88" t="s">
-        <v>153</v>
+        <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F88" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G88" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -3791,7 +3788,7 @@
         <v>42749</v>
       </c>
       <c r="C89" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D89" t="s">
         <v>153</v>
@@ -3808,30 +3805,30 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B90" s="3">
         <v>42749</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D90" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="E90" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F90" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G90" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B91" s="3">
         <v>42749</v>
@@ -3840,21 +3837,24 @@
         <v>8</v>
       </c>
       <c r="D91" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E91" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F91" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="G91" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B92" s="3">
-        <v>42750</v>
+        <v>42749</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -3863,15 +3863,15 @@
         <v>9</v>
       </c>
       <c r="E92" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F92" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B93" s="3">
         <v>42750</v>
@@ -3880,18 +3880,18 @@
         <v>8</v>
       </c>
       <c r="D93" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="E93" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F93" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B94" s="3">
         <v>42750</v>
@@ -3900,24 +3900,21 @@
         <v>8</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="E94" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F94" t="s">
-        <v>172</v>
-      </c>
-      <c r="G94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B95" s="3">
-        <v>42751</v>
+        <v>42750</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -3926,21 +3923,21 @@
         <v>9</v>
       </c>
       <c r="E95" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F95" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G95" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>177</v>
+        <v>351</v>
       </c>
       <c r="B96" s="3">
-        <v>42751</v>
+        <v>42750</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -3949,78 +3946,78 @@
         <v>21</v>
       </c>
       <c r="E96" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="F96" t="s">
-        <v>179</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>364</v>
       </c>
       <c r="B97" s="3">
-        <v>42751</v>
+        <v>42750</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E97" t="s">
-        <v>181</v>
+        <v>365</v>
       </c>
       <c r="F97" t="s">
-        <v>182</v>
-      </c>
-      <c r="G97" t="s">
-        <v>176</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>183</v>
+        <v>498</v>
       </c>
       <c r="B98" s="3">
-        <v>42751</v>
+        <v>42750</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
       </c>
       <c r="D98" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E98" t="s">
-        <v>184</v>
+        <v>499</v>
       </c>
       <c r="F98" t="s">
-        <v>185</v>
+        <v>500</v>
+      </c>
+      <c r="G98" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>510</v>
       </c>
       <c r="B99" s="3">
-        <v>42751</v>
+        <v>42750</v>
       </c>
       <c r="C99" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D99" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E99" t="s">
-        <v>184</v>
+        <v>511</v>
       </c>
       <c r="F99" t="s">
-        <v>185</v>
+        <v>512</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B100" s="3">
         <v>42751</v>
@@ -4032,10 +4029,10 @@
         <v>9</v>
       </c>
       <c r="E100" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="F100" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="G100" t="s">
         <v>176</v>
@@ -4043,116 +4040,116 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B101" s="3">
-        <v>42752</v>
+        <v>42751</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="E101" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F101" t="s">
-        <v>191</v>
-      </c>
-      <c r="G101" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B102" s="3">
-        <v>42752</v>
+        <v>42751</v>
       </c>
       <c r="C102" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D102" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="E102" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F102" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G102" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B103" s="3">
-        <v>42753</v>
+        <v>42751</v>
       </c>
       <c r="C103" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E103" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="F103" t="s">
-        <v>195</v>
-      </c>
-      <c r="G103" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="B104" s="3">
-        <v>42755</v>
+        <v>42751</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E104" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="F104" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="B105" s="3">
-        <v>42755</v>
+        <v>42751</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
       </c>
       <c r="E105" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="F105" t="s">
-        <v>213</v>
+        <v>188</v>
+      </c>
+      <c r="G105" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>214</v>
+        <v>329</v>
       </c>
       <c r="B106" s="3">
-        <v>42755</v>
+        <v>42751</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -4161,193 +4158,187 @@
         <v>63</v>
       </c>
       <c r="E106" t="s">
-        <v>215</v>
+        <v>330</v>
       </c>
       <c r="F106" t="s">
-        <v>216</v>
+        <v>331</v>
       </c>
       <c r="G106" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B107" s="3">
-        <v>42755</v>
+        <v>42751</v>
       </c>
       <c r="C107" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D107" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E107" t="s">
-        <v>218</v>
+        <v>330</v>
       </c>
       <c r="F107" t="s">
-        <v>219</v>
+        <v>331</v>
       </c>
       <c r="G107" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>217</v>
+        <v>446</v>
       </c>
       <c r="B108" s="3">
-        <v>42755</v>
+        <v>42751</v>
       </c>
       <c r="C108" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D108" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E108" t="s">
-        <v>218</v>
+        <v>447</v>
       </c>
       <c r="F108" t="s">
-        <v>219</v>
-      </c>
-      <c r="G108" t="s">
-        <v>220</v>
+        <v>448</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>217</v>
+        <v>160</v>
       </c>
       <c r="B109" s="3">
-        <v>42755</v>
+        <v>42751</v>
       </c>
       <c r="C109" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D109" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E109" t="s">
-        <v>218</v>
+        <v>504</v>
       </c>
       <c r="F109" t="s">
-        <v>219</v>
-      </c>
-      <c r="G109" t="s">
-        <v>220</v>
+        <v>505</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>217</v>
+        <v>506</v>
       </c>
       <c r="B110" s="3">
-        <v>42755</v>
+        <v>42751</v>
       </c>
       <c r="C110" t="s">
-        <v>221</v>
+        <v>8</v>
       </c>
       <c r="D110" t="s">
-        <v>21</v>
+        <v>507</v>
       </c>
       <c r="E110" t="s">
-        <v>218</v>
+        <v>508</v>
       </c>
       <c r="F110" t="s">
-        <v>219</v>
-      </c>
-      <c r="G110" t="s">
-        <v>220</v>
+        <v>509</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="B111" s="3">
-        <v>42762</v>
+        <v>42752</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
       </c>
       <c r="D111" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="E111" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="F111" t="s">
-        <v>224</v>
+        <v>191</v>
       </c>
       <c r="G111" t="s">
-        <v>122</v>
+        <v>192</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="B112" s="3">
-        <v>42762</v>
+        <v>42752</v>
       </c>
       <c r="C112" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D112" t="s">
-        <v>9</v>
+        <v>132</v>
       </c>
       <c r="E112" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="F112" t="s">
-        <v>227</v>
+        <v>191</v>
+      </c>
+      <c r="G112" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>225</v>
+        <v>326</v>
       </c>
       <c r="B113" s="3">
-        <v>42762</v>
+        <v>42752</v>
       </c>
       <c r="C113" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D113" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="E113" t="s">
-        <v>226</v>
+        <v>327</v>
       </c>
       <c r="F113" t="s">
-        <v>227</v>
+        <v>328</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B114" s="3">
-        <v>42761</v>
+        <v>42752</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D114" t="s">
-        <v>323</v>
+        <v>108</v>
       </c>
       <c r="E114" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="F114" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="B115" s="3">
         <v>42752</v>
@@ -4356,147 +4347,147 @@
         <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="E115" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="F115" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="B116" s="3">
         <v>42752</v>
       </c>
       <c r="C116" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D116" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="E116" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="F116" t="s">
-        <v>328</v>
+        <v>356</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>329</v>
+        <v>357</v>
       </c>
       <c r="B117" s="3">
-        <v>42751</v>
+        <v>42752</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
       </c>
       <c r="D117" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E117" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="F117" t="s">
-        <v>331</v>
-      </c>
-      <c r="G117" t="s">
-        <v>207</v>
+        <v>359</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
       <c r="B118" s="3">
-        <v>42751</v>
+        <v>42752</v>
       </c>
       <c r="C118" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D118" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E118" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="F118" t="s">
-        <v>331</v>
+        <v>362</v>
       </c>
       <c r="G118" t="s">
-        <v>207</v>
+        <v>363</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>332</v>
+        <v>493</v>
       </c>
       <c r="B119" s="3">
-        <v>42754</v>
+        <v>42752</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
       </c>
       <c r="D119" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E119" t="s">
-        <v>333</v>
+        <v>494</v>
       </c>
       <c r="F119" t="s">
-        <v>334</v>
+        <v>495</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>335</v>
+        <v>501</v>
       </c>
       <c r="B120" s="3">
-        <v>42756</v>
+        <v>42752</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
       </c>
       <c r="D120" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E120" t="s">
-        <v>336</v>
+        <v>502</v>
       </c>
       <c r="F120" t="s">
-        <v>337</v>
+        <v>503</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>338</v>
+        <v>193</v>
       </c>
       <c r="B121" s="3">
-        <v>42752</v>
+        <v>42753</v>
       </c>
       <c r="C121" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D121" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E121" t="s">
-        <v>339</v>
+        <v>194</v>
       </c>
       <c r="F121" t="s">
-        <v>340</v>
+        <v>195</v>
+      </c>
+      <c r="G121" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="B122" s="3">
-        <v>42755</v>
+        <v>42753</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
@@ -4505,61 +4496,55 @@
         <v>21</v>
       </c>
       <c r="E122" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="F122" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>344</v>
+        <v>396</v>
       </c>
       <c r="B123" s="3">
-        <v>42754</v>
+        <v>42753</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
       </c>
       <c r="D123" t="s">
-        <v>21</v>
+        <v>392</v>
       </c>
       <c r="E123" t="s">
-        <v>345</v>
+        <v>397</v>
       </c>
       <c r="F123" t="s">
-        <v>346</v>
-      </c>
-      <c r="G123" t="s">
-        <v>347</v>
+        <v>398</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>344</v>
+        <v>30</v>
       </c>
       <c r="B124" s="3">
-        <v>42754</v>
+        <v>42753</v>
       </c>
       <c r="C124" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E124" t="s">
-        <v>345</v>
+        <v>403</v>
       </c>
       <c r="F124" t="s">
-        <v>346</v>
-      </c>
-      <c r="G124" t="s">
-        <v>347</v>
+        <v>404</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>348</v>
+        <v>424</v>
       </c>
       <c r="B125" s="3">
         <v>42753</v>
@@ -4568,41 +4553,41 @@
         <v>8</v>
       </c>
       <c r="D125" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E125" t="s">
-        <v>349</v>
+        <v>425</v>
       </c>
       <c r="F125" t="s">
-        <v>350</v>
+        <v>426</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>351</v>
+        <v>461</v>
       </c>
       <c r="B126" s="3">
-        <v>42750</v>
+        <v>42753</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
       </c>
       <c r="D126" t="s">
-        <v>21</v>
+        <v>462</v>
       </c>
       <c r="E126" t="s">
-        <v>352</v>
+        <v>463</v>
       </c>
       <c r="F126" t="s">
-        <v>353</v>
+        <v>464</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="B127" s="3">
-        <v>42752</v>
+        <v>42754</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -4611,18 +4596,18 @@
         <v>21</v>
       </c>
       <c r="E127" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="F127" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="B128" s="3">
-        <v>42752</v>
+        <v>42754</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -4631,407 +4616,431 @@
         <v>21</v>
       </c>
       <c r="E128" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="F128" t="s">
-        <v>359</v>
+        <v>346</v>
+      </c>
+      <c r="G128" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B129" s="3">
-        <v>42752</v>
+        <v>42754</v>
       </c>
       <c r="C129" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D129" t="s">
         <v>21</v>
       </c>
       <c r="E129" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="F129" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="G129" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>364</v>
+        <v>379</v>
       </c>
       <c r="B130" s="3">
-        <v>42750</v>
+        <v>42754</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
       </c>
       <c r="D130" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E130" t="s">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="F130" t="s">
-        <v>366</v>
+        <v>381</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>367</v>
+        <v>490</v>
       </c>
       <c r="B131" s="3">
-        <v>42761</v>
+        <v>42754</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
       </c>
       <c r="D131" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E131" t="s">
-        <v>368</v>
+        <v>491</v>
       </c>
       <c r="F131" t="s">
-        <v>369</v>
+        <v>492</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>370</v>
+        <v>315</v>
       </c>
       <c r="B132" s="3">
-        <v>42760</v>
+        <v>42754</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
       </c>
       <c r="D132" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E132" t="s">
-        <v>371</v>
+        <v>496</v>
       </c>
       <c r="F132" t="s">
-        <v>372</v>
+        <v>497</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>370</v>
+        <v>211</v>
       </c>
       <c r="B133" s="3">
-        <v>42760</v>
+        <v>42755</v>
       </c>
       <c r="C133" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D133" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E133" t="s">
-        <v>371</v>
+        <v>212</v>
       </c>
       <c r="F133" t="s">
-        <v>372</v>
+        <v>213</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>373</v>
+        <v>211</v>
       </c>
       <c r="B134" s="3">
-        <v>42759</v>
-      </c>
-      <c r="C134" t="s">
-        <v>8</v>
+        <v>42755</v>
       </c>
       <c r="D134" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E134" t="s">
-        <v>374</v>
+        <v>212</v>
       </c>
       <c r="F134" t="s">
-        <v>375</v>
+        <v>213</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>373</v>
+        <v>214</v>
       </c>
       <c r="B135" s="3">
-        <v>42759</v>
+        <v>42755</v>
       </c>
       <c r="C135" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D135" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E135" t="s">
-        <v>374</v>
+        <v>215</v>
       </c>
       <c r="F135" t="s">
-        <v>375</v>
+        <v>216</v>
+      </c>
+      <c r="G135" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>376</v>
+        <v>217</v>
       </c>
       <c r="B136" s="3">
-        <v>42758</v>
+        <v>42755</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
       </c>
       <c r="D136" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E136" t="s">
-        <v>377</v>
+        <v>218</v>
       </c>
       <c r="F136" t="s">
-        <v>378</v>
+        <v>219</v>
+      </c>
+      <c r="G136" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>379</v>
+        <v>217</v>
       </c>
       <c r="B137" s="3">
-        <v>42754</v>
+        <v>42755</v>
       </c>
       <c r="C137" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D137" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E137" t="s">
-        <v>380</v>
+        <v>218</v>
       </c>
       <c r="F137" t="s">
-        <v>381</v>
+        <v>219</v>
+      </c>
+      <c r="G137" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>382</v>
+        <v>217</v>
       </c>
       <c r="B138" s="3">
-        <v>42766</v>
+        <v>42755</v>
       </c>
       <c r="C138" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D138" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E138" t="s">
-        <v>383</v>
+        <v>218</v>
       </c>
       <c r="F138" t="s">
-        <v>384</v>
+        <v>219</v>
+      </c>
+      <c r="G138" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>387</v>
+        <v>217</v>
       </c>
       <c r="B139" s="3">
-        <v>42760</v>
+        <v>42755</v>
       </c>
       <c r="C139" t="s">
-        <v>8</v>
+        <v>221</v>
       </c>
       <c r="D139" t="s">
-        <v>388</v>
+        <v>21</v>
       </c>
       <c r="E139" t="s">
-        <v>389</v>
+        <v>218</v>
       </c>
       <c r="F139" t="s">
-        <v>390</v>
+        <v>219</v>
+      </c>
+      <c r="G139" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>391</v>
+        <v>341</v>
       </c>
       <c r="B140" s="3">
         <v>42755</v>
       </c>
       <c r="C140" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D140" t="s">
-        <v>392</v>
+        <v>21</v>
       </c>
       <c r="E140" t="s">
-        <v>393</v>
+        <v>342</v>
       </c>
       <c r="F140" t="s">
-        <v>394</v>
-      </c>
-      <c r="G140" t="s">
-        <v>395</v>
+        <v>343</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B141" s="3">
-        <v>42753</v>
+        <v>42755</v>
       </c>
       <c r="C141" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D141" t="s">
         <v>392</v>
       </c>
       <c r="E141" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F141" t="s">
-        <v>398</v>
+        <v>394</v>
+      </c>
+      <c r="G141" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>399</v>
+        <v>265</v>
       </c>
       <c r="B142" s="3">
-        <v>42757</v>
+        <v>42755</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
       </c>
       <c r="D142" t="s">
-        <v>400</v>
+        <v>9</v>
       </c>
       <c r="E142" t="s">
-        <v>401</v>
+        <v>472</v>
       </c>
       <c r="F142" t="s">
-        <v>402</v>
+        <v>473</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>30</v>
+        <v>265</v>
       </c>
       <c r="B143" s="3">
-        <v>42753</v>
+        <v>42755</v>
       </c>
       <c r="C143" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D143" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E143" t="s">
-        <v>403</v>
+        <v>472</v>
       </c>
       <c r="F143" t="s">
-        <v>404</v>
+        <v>473</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>12</v>
+        <v>474</v>
       </c>
       <c r="B144" s="3">
-        <v>42736</v>
+        <v>42755</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
       </c>
       <c r="D144" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E144" t="s">
-        <v>405</v>
+        <v>475</v>
       </c>
       <c r="F144" t="s">
-        <v>406</v>
+        <v>476</v>
+      </c>
+      <c r="G144" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>318</v>
+        <v>474</v>
       </c>
       <c r="B145" s="3">
-        <v>42762</v>
+        <v>42755</v>
       </c>
       <c r="C145" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D145" t="s">
-        <v>319</v>
+        <v>9</v>
       </c>
       <c r="E145" t="s">
-        <v>407</v>
+        <v>475</v>
       </c>
       <c r="F145" t="s">
-        <v>408</v>
+        <v>476</v>
+      </c>
+      <c r="G145" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>385</v>
+        <v>477</v>
       </c>
       <c r="B146" s="3">
-        <v>42762</v>
+        <v>42755</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
       </c>
       <c r="D146" t="s">
-        <v>386</v>
+        <v>9</v>
       </c>
       <c r="E146" t="s">
-        <v>409</v>
+        <v>478</v>
       </c>
       <c r="F146" t="s">
-        <v>410</v>
+        <v>479</v>
+      </c>
+      <c r="G146" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>411</v>
+        <v>477</v>
       </c>
       <c r="B147" s="3">
-        <v>42762</v>
+        <v>42755</v>
       </c>
       <c r="C147" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D147" t="s">
-        <v>412</v>
+        <v>9</v>
       </c>
       <c r="E147" t="s">
-        <v>413</v>
+        <v>478</v>
       </c>
       <c r="F147" t="s">
-        <v>414</v>
+        <v>479</v>
       </c>
       <c r="G147" t="s">
-        <v>415</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>416</v>
+        <v>69</v>
       </c>
       <c r="B148" s="3">
-        <v>42761</v>
+        <v>42755</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -5040,58 +5049,58 @@
         <v>9</v>
       </c>
       <c r="E148" t="s">
-        <v>417</v>
+        <v>485</v>
       </c>
       <c r="F148" t="s">
-        <v>418</v>
+        <v>486</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>367</v>
+        <v>487</v>
       </c>
       <c r="B149" s="3">
-        <v>42761</v>
+        <v>42755</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
       </c>
       <c r="D149" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E149" t="s">
-        <v>368</v>
+        <v>488</v>
       </c>
       <c r="F149" t="s">
-        <v>369</v>
+        <v>489</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="B150" s="3">
-        <v>42761</v>
+        <v>42756</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
       </c>
       <c r="D150" t="s">
-        <v>323</v>
+        <v>21</v>
       </c>
       <c r="E150" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="F150" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>231</v>
+        <v>480</v>
       </c>
       <c r="B151" s="3">
-        <v>42761</v>
+        <v>42756</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
@@ -5100,58 +5109,61 @@
         <v>9</v>
       </c>
       <c r="E151" t="s">
-        <v>419</v>
+        <v>480</v>
       </c>
       <c r="F151" t="s">
-        <v>420</v>
+        <v>481</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>421</v>
+        <v>482</v>
       </c>
       <c r="B152" s="3">
-        <v>42761</v>
+        <v>42756</v>
       </c>
       <c r="C152" t="s">
         <v>8</v>
       </c>
       <c r="D152" t="s">
-        <v>241</v>
+        <v>9</v>
       </c>
       <c r="E152" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="F152" t="s">
-        <v>423</v>
+        <v>484</v>
+      </c>
+      <c r="G152" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="B153" s="3">
-        <v>42753</v>
+        <v>42757</v>
       </c>
       <c r="C153" t="s">
         <v>8</v>
       </c>
       <c r="D153" t="s">
-        <v>9</v>
+        <v>400</v>
       </c>
       <c r="E153" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="F153" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="B154" s="3">
-        <v>42760</v>
+        <v>42757</v>
       </c>
       <c r="C154" t="s">
         <v>8</v>
@@ -5160,84 +5172,87 @@
         <v>9</v>
       </c>
       <c r="E154" t="s">
-        <v>428</v>
+        <v>450</v>
       </c>
       <c r="F154" t="s">
-        <v>429</v>
-      </c>
-      <c r="G154" t="s">
-        <v>265</v>
+        <v>451</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="B155" s="3">
-        <v>42760</v>
+        <v>42757</v>
       </c>
       <c r="C155" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D155" t="s">
-        <v>9</v>
+        <v>453</v>
       </c>
       <c r="E155" t="s">
-        <v>428</v>
+        <v>454</v>
       </c>
       <c r="F155" t="s">
-        <v>429</v>
+        <v>455</v>
       </c>
       <c r="G155" t="s">
-        <v>265</v>
+        <v>456</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>370</v>
+        <v>452</v>
       </c>
       <c r="B156" s="3">
-        <v>42760</v>
+        <v>42757</v>
       </c>
       <c r="C156" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D156" t="s">
-        <v>26</v>
+        <v>453</v>
       </c>
       <c r="E156" t="s">
-        <v>371</v>
+        <v>454</v>
       </c>
       <c r="F156" t="s">
-        <v>372</v>
+        <v>455</v>
+      </c>
+      <c r="G156" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>370</v>
+        <v>465</v>
       </c>
       <c r="B157" s="3">
-        <v>42760</v>
+        <v>42757</v>
       </c>
       <c r="C157" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D157" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E157" t="s">
-        <v>371</v>
+        <v>466</v>
       </c>
       <c r="F157" t="s">
-        <v>372</v>
+        <v>467</v>
+      </c>
+      <c r="G157" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>430</v>
+        <v>69</v>
       </c>
       <c r="B158" s="3">
-        <v>42765</v>
+        <v>42757</v>
       </c>
       <c r="C158" t="s">
         <v>8</v>
@@ -5246,84 +5261,78 @@
         <v>9</v>
       </c>
       <c r="E158" t="s">
-        <v>430</v>
+        <v>468</v>
       </c>
       <c r="F158" t="s">
-        <v>431</v>
-      </c>
-      <c r="G158" t="s">
-        <v>432</v>
+        <v>469</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>373</v>
+        <v>69</v>
       </c>
       <c r="B159" s="3">
-        <v>42759</v>
+        <v>42757</v>
       </c>
       <c r="C159" t="s">
         <v>8</v>
       </c>
       <c r="D159" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E159" t="s">
-        <v>374</v>
+        <v>470</v>
       </c>
       <c r="F159" t="s">
-        <v>375</v>
+        <v>471</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B160" s="3">
-        <v>42759</v>
+        <v>42758</v>
       </c>
       <c r="C160" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="D160" t="s">
         <v>26</v>
       </c>
       <c r="E160" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="F160" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="B161" s="3">
-        <v>42762</v>
+        <v>42758</v>
       </c>
       <c r="C161" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D161" t="s">
         <v>9</v>
       </c>
       <c r="E161" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="F161" t="s">
-        <v>435</v>
-      </c>
-      <c r="G161" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>433</v>
+        <v>457</v>
       </c>
       <c r="B162" s="3">
-        <v>42762</v>
+        <v>42758</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
@@ -5332,78 +5341,78 @@
         <v>9</v>
       </c>
       <c r="E162" t="s">
-        <v>434</v>
+        <v>458</v>
       </c>
       <c r="F162" t="s">
-        <v>435</v>
+        <v>459</v>
       </c>
       <c r="G162" t="s">
-        <v>436</v>
+        <v>460</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B163" s="3">
-        <v>42760</v>
+        <v>42759</v>
       </c>
       <c r="C163" t="s">
         <v>8</v>
       </c>
       <c r="D163" t="s">
-        <v>388</v>
+        <v>26</v>
       </c>
       <c r="E163" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="F163" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>326</v>
+        <v>373</v>
       </c>
       <c r="B164" s="3">
-        <v>42752</v>
+        <v>42759</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D164" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="E164" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
       <c r="F164" t="s">
-        <v>328</v>
+        <v>375</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>326</v>
+        <v>437</v>
       </c>
       <c r="B165" s="3">
-        <v>42752</v>
+        <v>42759</v>
       </c>
       <c r="C165" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D165" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="E165" t="s">
-        <v>327</v>
+        <v>438</v>
       </c>
       <c r="F165" t="s">
-        <v>328</v>
+        <v>439</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="B166" s="3">
         <v>42759</v>
@@ -5415,158 +5424,164 @@
         <v>9</v>
       </c>
       <c r="E166" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="F166" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>440</v>
+        <v>370</v>
       </c>
       <c r="B167" s="3">
-        <v>42759</v>
+        <v>42760</v>
       </c>
       <c r="C167" t="s">
         <v>8</v>
       </c>
       <c r="D167" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E167" t="s">
-        <v>441</v>
+        <v>371</v>
       </c>
       <c r="F167" t="s">
-        <v>442</v>
+        <v>372</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>332</v>
+        <v>370</v>
       </c>
       <c r="B168" s="3">
-        <v>42754</v>
+        <v>42760</v>
       </c>
       <c r="C168" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D168" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E168" t="s">
-        <v>333</v>
+        <v>371</v>
       </c>
       <c r="F168" t="s">
-        <v>334</v>
+        <v>372</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>335</v>
+        <v>387</v>
       </c>
       <c r="B169" s="3">
-        <v>42756</v>
+        <v>42760</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>
       </c>
       <c r="D169" t="s">
-        <v>21</v>
+        <v>388</v>
       </c>
       <c r="E169" t="s">
-        <v>336</v>
+        <v>389</v>
       </c>
       <c r="F169" t="s">
-        <v>337</v>
+        <v>390</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>338</v>
+        <v>427</v>
       </c>
       <c r="B170" s="3">
-        <v>42752</v>
+        <v>42760</v>
       </c>
       <c r="C170" t="s">
         <v>8</v>
       </c>
       <c r="D170" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E170" t="s">
-        <v>339</v>
+        <v>428</v>
       </c>
       <c r="F170" t="s">
-        <v>340</v>
+        <v>429</v>
+      </c>
+      <c r="G170" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="B171" s="3">
-        <v>42758</v>
+        <v>42760</v>
       </c>
       <c r="C171" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D171" t="s">
         <v>9</v>
       </c>
       <c r="E171" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="F171" t="s">
-        <v>445</v>
+        <v>429</v>
+      </c>
+      <c r="G171" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>376</v>
+        <v>322</v>
       </c>
       <c r="B172" s="3">
-        <v>42758</v>
+        <v>42761</v>
       </c>
       <c r="C172" t="s">
         <v>8</v>
       </c>
       <c r="D172" t="s">
-        <v>26</v>
+        <v>323</v>
       </c>
       <c r="E172" t="s">
-        <v>377</v>
+        <v>324</v>
       </c>
       <c r="F172" t="s">
-        <v>378</v>
+        <v>325</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>446</v>
+        <v>367</v>
       </c>
       <c r="B173" s="3">
-        <v>42751</v>
+        <v>42761</v>
       </c>
       <c r="C173" t="s">
         <v>8</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E173" t="s">
-        <v>447</v>
+        <v>368</v>
       </c>
       <c r="F173" t="s">
-        <v>448</v>
+        <v>369</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>449</v>
+        <v>416</v>
       </c>
       <c r="B174" s="3">
-        <v>42757</v>
+        <v>42761</v>
       </c>
       <c r="C174" t="s">
         <v>8</v>
@@ -5575,84 +5590,81 @@
         <v>9</v>
       </c>
       <c r="E174" t="s">
-        <v>450</v>
+        <v>417</v>
       </c>
       <c r="F174" t="s">
-        <v>451</v>
+        <v>418</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>452</v>
+        <v>231</v>
       </c>
       <c r="B175" s="3">
-        <v>42757</v>
+        <v>42761</v>
       </c>
       <c r="C175" t="s">
         <v>8</v>
       </c>
       <c r="D175" t="s">
-        <v>453</v>
+        <v>9</v>
       </c>
       <c r="E175" t="s">
-        <v>454</v>
+        <v>419</v>
       </c>
       <c r="F175" t="s">
-        <v>455</v>
-      </c>
-      <c r="G175" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="B176" s="3">
-        <v>42757</v>
+        <v>42761</v>
       </c>
       <c r="C176" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D176" t="s">
-        <v>453</v>
+        <v>241</v>
       </c>
       <c r="E176" t="s">
-        <v>454</v>
+        <v>422</v>
       </c>
       <c r="F176" t="s">
-        <v>455</v>
-      </c>
-      <c r="G176" t="s">
-        <v>456</v>
+        <v>423</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>399</v>
+        <v>222</v>
       </c>
       <c r="B177" s="3">
-        <v>42757</v>
+        <v>42762</v>
       </c>
       <c r="C177" t="s">
         <v>8</v>
       </c>
       <c r="D177" t="s">
-        <v>400</v>
+        <v>63</v>
       </c>
       <c r="E177" t="s">
-        <v>401</v>
+        <v>223</v>
       </c>
       <c r="F177" t="s">
-        <v>402</v>
+        <v>224</v>
+      </c>
+      <c r="G177" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>457</v>
+        <v>225</v>
       </c>
       <c r="B178" s="3">
-        <v>42758</v>
+        <v>42762</v>
       </c>
       <c r="C178" t="s">
         <v>8</v>
@@ -5661,124 +5673,124 @@
         <v>9</v>
       </c>
       <c r="E178" t="s">
-        <v>458</v>
+        <v>226</v>
       </c>
       <c r="F178" t="s">
-        <v>459</v>
-      </c>
-      <c r="G178" t="s">
-        <v>460</v>
+        <v>227</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>461</v>
+        <v>225</v>
       </c>
       <c r="B179" s="3">
-        <v>42753</v>
+        <v>42762</v>
       </c>
       <c r="C179" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D179" t="s">
-        <v>462</v>
+        <v>9</v>
       </c>
       <c r="E179" t="s">
-        <v>463</v>
+        <v>226</v>
       </c>
       <c r="F179" t="s">
-        <v>464</v>
+        <v>227</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="B180" s="3">
-        <v>42755</v>
+        <v>42762</v>
       </c>
       <c r="C180" t="s">
         <v>8</v>
       </c>
       <c r="D180" t="s">
-        <v>21</v>
+        <v>319</v>
       </c>
       <c r="E180" t="s">
-        <v>342</v>
+        <v>407</v>
       </c>
       <c r="F180" t="s">
-        <v>343</v>
+        <v>408</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>465</v>
+        <v>385</v>
       </c>
       <c r="B181" s="3">
-        <v>42757</v>
+        <v>42762</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>9</v>
+        <v>386</v>
       </c>
       <c r="E181" t="s">
-        <v>466</v>
+        <v>409</v>
       </c>
       <c r="F181" t="s">
-        <v>467</v>
-      </c>
-      <c r="G181" t="s">
-        <v>60</v>
+        <v>410</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>69</v>
+        <v>411</v>
       </c>
       <c r="B182" s="3">
-        <v>42757</v>
+        <v>42762</v>
       </c>
       <c r="C182" t="s">
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>9</v>
+        <v>412</v>
       </c>
       <c r="E182" t="s">
-        <v>468</v>
+        <v>413</v>
       </c>
       <c r="F182" t="s">
-        <v>469</v>
+        <v>414</v>
+      </c>
+      <c r="G182" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>69</v>
+        <v>433</v>
       </c>
       <c r="B183" s="3">
-        <v>42757</v>
+        <v>42762</v>
       </c>
       <c r="C183" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D183" t="s">
         <v>9</v>
       </c>
       <c r="E183" t="s">
-        <v>470</v>
+        <v>434</v>
       </c>
       <c r="F183" t="s">
-        <v>471</v>
+        <v>435</v>
+      </c>
+      <c r="G183" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>265</v>
+        <v>433</v>
       </c>
       <c r="B184" s="3">
-        <v>42755</v>
+        <v>42762</v>
       </c>
       <c r="C184" t="s">
         <v>8</v>
@@ -5787,691 +5799,151 @@
         <v>9</v>
       </c>
       <c r="E184" t="s">
-        <v>472</v>
+        <v>434</v>
       </c>
       <c r="F184" t="s">
-        <v>473</v>
+        <v>435</v>
+      </c>
+      <c r="G184" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>265</v>
+        <v>430</v>
       </c>
       <c r="B185" s="3">
-        <v>42755</v>
+        <v>42765</v>
       </c>
       <c r="C185" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="D185" t="s">
         <v>9</v>
       </c>
       <c r="E185" t="s">
-        <v>472</v>
+        <v>430</v>
       </c>
       <c r="F185" t="s">
-        <v>473</v>
+        <v>431</v>
+      </c>
+      <c r="G185" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>474</v>
+        <v>382</v>
       </c>
       <c r="B186" s="3">
-        <v>42755</v>
+        <v>42766</v>
       </c>
       <c r="C186" t="s">
         <v>8</v>
       </c>
       <c r="D186" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E186" t="s">
-        <v>475</v>
+        <v>383</v>
       </c>
       <c r="F186" t="s">
-        <v>476</v>
-      </c>
-      <c r="G186" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>474</v>
-      </c>
-      <c r="B187" s="3">
-        <v>42755</v>
-      </c>
-      <c r="C187" t="s">
-        <v>62</v>
-      </c>
-      <c r="D187" t="s">
-        <v>9</v>
-      </c>
-      <c r="E187" t="s">
-        <v>475</v>
-      </c>
-      <c r="F187" t="s">
-        <v>476</v>
-      </c>
-      <c r="G187" t="s">
-        <v>265</v>
-      </c>
+      <c r="B187"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>477</v>
-      </c>
-      <c r="B188" s="3">
-        <v>42755</v>
-      </c>
-      <c r="C188" t="s">
-        <v>8</v>
-      </c>
-      <c r="D188" t="s">
-        <v>9</v>
-      </c>
-      <c r="E188" t="s">
-        <v>478</v>
-      </c>
-      <c r="F188" t="s">
-        <v>479</v>
-      </c>
-      <c r="G188" t="s">
-        <v>265</v>
-      </c>
+      <c r="B188"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>477</v>
-      </c>
-      <c r="B189" s="3">
-        <v>42755</v>
-      </c>
-      <c r="C189" t="s">
-        <v>62</v>
-      </c>
-      <c r="D189" t="s">
-        <v>9</v>
-      </c>
-      <c r="E189" t="s">
-        <v>478</v>
-      </c>
-      <c r="F189" t="s">
-        <v>479</v>
-      </c>
-      <c r="G189" t="s">
-        <v>265</v>
-      </c>
+      <c r="B189"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
-        <v>480</v>
-      </c>
-      <c r="B190" s="3">
-        <v>42756</v>
-      </c>
-      <c r="C190" t="s">
-        <v>8</v>
-      </c>
-      <c r="D190" t="s">
-        <v>9</v>
-      </c>
-      <c r="E190" t="s">
-        <v>480</v>
-      </c>
-      <c r="F190" t="s">
-        <v>481</v>
-      </c>
+      <c r="B190"/>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>482</v>
-      </c>
-      <c r="B191" s="3">
-        <v>42756</v>
-      </c>
-      <c r="C191" t="s">
-        <v>8</v>
-      </c>
-      <c r="D191" t="s">
-        <v>9</v>
-      </c>
-      <c r="E191" t="s">
-        <v>483</v>
-      </c>
-      <c r="F191" t="s">
-        <v>484</v>
-      </c>
-      <c r="G191" t="s">
-        <v>160</v>
-      </c>
+      <c r="B191"/>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>69</v>
-      </c>
-      <c r="B192" s="3">
-        <v>42755</v>
-      </c>
-      <c r="C192" t="s">
-        <v>8</v>
-      </c>
-      <c r="D192" t="s">
-        <v>9</v>
-      </c>
-      <c r="E192" t="s">
-        <v>485</v>
-      </c>
-      <c r="F192" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>391</v>
-      </c>
-      <c r="B193" s="3">
-        <v>42755</v>
-      </c>
-      <c r="C193" t="s">
-        <v>104</v>
-      </c>
-      <c r="D193" t="s">
-        <v>392</v>
-      </c>
-      <c r="E193" t="s">
-        <v>393</v>
-      </c>
-      <c r="F193" t="s">
-        <v>394</v>
-      </c>
-      <c r="G193" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>487</v>
-      </c>
-      <c r="B194" s="3">
-        <v>42755</v>
-      </c>
-      <c r="C194" t="s">
-        <v>8</v>
-      </c>
-      <c r="D194" t="s">
-        <v>9</v>
-      </c>
-      <c r="E194" t="s">
-        <v>488</v>
-      </c>
-      <c r="F194" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>379</v>
-      </c>
-      <c r="B195" s="3">
-        <v>42754</v>
-      </c>
-      <c r="C195" t="s">
-        <v>8</v>
-      </c>
-      <c r="D195" t="s">
-        <v>26</v>
-      </c>
-      <c r="E195" t="s">
-        <v>380</v>
-      </c>
-      <c r="F195" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>490</v>
-      </c>
-      <c r="B196" s="3">
-        <v>42754</v>
-      </c>
-      <c r="C196" t="s">
-        <v>8</v>
-      </c>
-      <c r="D196" t="s">
-        <v>42</v>
-      </c>
-      <c r="E196" t="s">
-        <v>491</v>
-      </c>
-      <c r="F196" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
-        <v>344</v>
-      </c>
-      <c r="B197" s="3">
-        <v>42754</v>
-      </c>
-      <c r="C197" t="s">
-        <v>8</v>
-      </c>
-      <c r="D197" t="s">
-        <v>21</v>
-      </c>
-      <c r="E197" t="s">
-        <v>345</v>
-      </c>
-      <c r="F197" t="s">
-        <v>346</v>
-      </c>
-      <c r="G197" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>344</v>
-      </c>
-      <c r="B198" s="3">
-        <v>42754</v>
-      </c>
-      <c r="C198" t="s">
-        <v>56</v>
-      </c>
-      <c r="D198" t="s">
-        <v>21</v>
-      </c>
-      <c r="E198" t="s">
-        <v>345</v>
-      </c>
-      <c r="F198" t="s">
-        <v>346</v>
-      </c>
-      <c r="G198" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
-        <v>493</v>
-      </c>
-      <c r="B199" s="3">
-        <v>42752</v>
-      </c>
-      <c r="C199" t="s">
-        <v>8</v>
-      </c>
-      <c r="D199" t="s">
-        <v>9</v>
-      </c>
-      <c r="E199" t="s">
-        <v>494</v>
-      </c>
-      <c r="F199" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>315</v>
-      </c>
-      <c r="B200" s="3">
-        <v>42754</v>
-      </c>
-      <c r="C200" t="s">
-        <v>8</v>
-      </c>
-      <c r="D200" t="s">
-        <v>9</v>
-      </c>
-      <c r="E200" t="s">
-        <v>496</v>
-      </c>
-      <c r="F200" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>348</v>
-      </c>
-      <c r="B201" s="3">
-        <v>42753</v>
-      </c>
-      <c r="C201" t="s">
-        <v>8</v>
-      </c>
-      <c r="D201" t="s">
-        <v>21</v>
-      </c>
-      <c r="E201" t="s">
-        <v>349</v>
-      </c>
-      <c r="F201" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
-        <v>498</v>
-      </c>
-      <c r="B202" s="3">
-        <v>42750</v>
-      </c>
-      <c r="C202" t="s">
-        <v>8</v>
-      </c>
-      <c r="D202" t="s">
-        <v>9</v>
-      </c>
-      <c r="E202" t="s">
-        <v>499</v>
-      </c>
-      <c r="F202" t="s">
-        <v>500</v>
-      </c>
-      <c r="G202" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>351</v>
-      </c>
-      <c r="B203" s="3">
-        <v>42750</v>
-      </c>
-      <c r="C203" t="s">
-        <v>8</v>
-      </c>
-      <c r="D203" t="s">
-        <v>21</v>
-      </c>
-      <c r="E203" t="s">
-        <v>352</v>
-      </c>
-      <c r="F203" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>396</v>
-      </c>
-      <c r="B204" s="3">
-        <v>42753</v>
-      </c>
-      <c r="C204" t="s">
-        <v>8</v>
-      </c>
-      <c r="D204" t="s">
-        <v>392</v>
-      </c>
-      <c r="E204" t="s">
-        <v>397</v>
-      </c>
-      <c r="F204" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
-        <v>501</v>
-      </c>
-      <c r="B205" s="3">
-        <v>42752</v>
-      </c>
-      <c r="C205" t="s">
-        <v>8</v>
-      </c>
-      <c r="D205" t="s">
-        <v>9</v>
-      </c>
-      <c r="E205" t="s">
-        <v>502</v>
-      </c>
-      <c r="F205" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>354</v>
-      </c>
-      <c r="B206" s="3">
-        <v>42752</v>
-      </c>
-      <c r="C206" t="s">
-        <v>8</v>
-      </c>
-      <c r="D206" t="s">
-        <v>21</v>
-      </c>
-      <c r="E206" t="s">
-        <v>355</v>
-      </c>
-      <c r="F206" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
-        <v>160</v>
-      </c>
-      <c r="B207" s="3">
-        <v>42751</v>
-      </c>
-      <c r="C207" t="s">
-        <v>8</v>
-      </c>
-      <c r="D207" t="s">
-        <v>9</v>
-      </c>
-      <c r="E207" t="s">
-        <v>504</v>
-      </c>
-      <c r="F207" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>357</v>
-      </c>
-      <c r="B208" s="3">
-        <v>42752</v>
-      </c>
-      <c r="C208" t="s">
-        <v>8</v>
-      </c>
-      <c r="D208" t="s">
-        <v>21</v>
-      </c>
-      <c r="E208" t="s">
-        <v>358</v>
-      </c>
-      <c r="F208" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
-        <v>360</v>
-      </c>
-      <c r="B209" s="3">
-        <v>42752</v>
-      </c>
-      <c r="C209" t="s">
-        <v>8</v>
-      </c>
-      <c r="D209" t="s">
-        <v>21</v>
-      </c>
-      <c r="E209" t="s">
-        <v>361</v>
-      </c>
-      <c r="F209" t="s">
-        <v>362</v>
-      </c>
-      <c r="G209" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>382</v>
-      </c>
-      <c r="B210" s="3">
-        <v>42766</v>
-      </c>
-      <c r="C210" t="s">
-        <v>8</v>
-      </c>
-      <c r="D210" t="s">
-        <v>26</v>
-      </c>
-      <c r="E210" t="s">
-        <v>383</v>
-      </c>
-      <c r="F210" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
-        <v>329</v>
-      </c>
-      <c r="B211" s="3">
-        <v>42751</v>
-      </c>
-      <c r="C211" t="s">
-        <v>8</v>
-      </c>
-      <c r="D211" t="s">
-        <v>63</v>
-      </c>
-      <c r="E211" t="s">
-        <v>330</v>
-      </c>
-      <c r="F211" t="s">
-        <v>331</v>
-      </c>
-      <c r="G211" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>329</v>
-      </c>
-      <c r="B212" s="3">
-        <v>42751</v>
-      </c>
-      <c r="C212" t="s">
-        <v>62</v>
-      </c>
-      <c r="D212" t="s">
-        <v>63</v>
-      </c>
-      <c r="E212" t="s">
-        <v>330</v>
-      </c>
-      <c r="F212" t="s">
-        <v>331</v>
-      </c>
-      <c r="G212" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>506</v>
-      </c>
-      <c r="B213" s="3">
-        <v>42751</v>
-      </c>
-      <c r="C213" t="s">
-        <v>8</v>
-      </c>
-      <c r="D213" t="s">
-        <v>507</v>
-      </c>
-      <c r="E213" t="s">
-        <v>508</v>
-      </c>
-      <c r="F213" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>510</v>
-      </c>
-      <c r="B214" s="3">
-        <v>42750</v>
-      </c>
-      <c r="C214" t="s">
-        <v>8</v>
-      </c>
-      <c r="D214" t="s">
-        <v>9</v>
-      </c>
-      <c r="E214" t="s">
-        <v>511</v>
-      </c>
-      <c r="F214" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>364</v>
-      </c>
-      <c r="B215" s="3">
-        <v>42750</v>
-      </c>
-      <c r="C215" t="s">
-        <v>8</v>
-      </c>
-      <c r="D215" t="s">
-        <v>21</v>
-      </c>
-      <c r="E215" t="s">
-        <v>365</v>
-      </c>
-      <c r="F215" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>12</v>
-      </c>
-      <c r="B216" s="3">
-        <v>42736</v>
-      </c>
-      <c r="C216" t="s">
-        <v>8</v>
-      </c>
-      <c r="D216" t="s">
-        <v>13</v>
-      </c>
-      <c r="E216" t="s">
-        <v>405</v>
-      </c>
-      <c r="F216" t="s">
-        <v>406</v>
-      </c>
+      <c r="B192"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B193"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B194"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B195"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B196"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B197"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B198"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B199"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B200"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B201"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B202"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B203"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B204"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B205"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B206"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B207"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B208"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B209"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B210"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B211"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B212"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B213"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B214"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B215"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B216"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H216">
-    <sortState ref="A2:H113">
+    <sortState ref="A2:G216">
       <sortCondition ref="B1:B113"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
updated to automatic run and upload to drive
</commit_message>
<xml_diff>
--- a/bandcamp_januari_01-02-2017.xlsx
+++ b/bandcamp_januari_01-02-2017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2693,21 +2693,9 @@
     <t>xaero</t>
   </si>
   <si>
-    <t>artiest</t>
-  </si>
-  <si>
-    <t>datum</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
-    <t>locatie</t>
-  </si>
-  <si>
-    <t>titel</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -2802,6 +2790,18 @@
   </si>
   <si>
     <t>Charlotte Haesen</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -6555,7 +6555,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A148" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" showAll="0">
@@ -7156,6 +7156,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
@@ -7458,7 +7461,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -8178,12 +8181,12 @@
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -8375,7 +8378,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="C15" t="b">
         <f t="shared" si="0"/>
@@ -8540,7 +8543,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="C29" t="b">
         <f t="shared" si="0"/>
@@ -9077,7 +9080,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="C74" t="b">
         <f t="shared" si="1"/>
@@ -9086,7 +9089,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="C75" t="b">
         <f t="shared" si="1"/>
@@ -9095,7 +9098,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="C76" t="b">
         <f t="shared" si="1"/>
@@ -9104,7 +9107,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C77" t="b">
         <f t="shared" si="1"/>
@@ -9113,7 +9116,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C78" t="b">
         <f t="shared" si="1"/>
@@ -9122,7 +9125,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="C79" t="b">
         <f t="shared" si="1"/>
@@ -9131,7 +9134,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="C80" t="b">
         <f t="shared" si="1"/>
@@ -9140,7 +9143,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="C81" t="b">
         <f t="shared" si="1"/>
@@ -9149,7 +9152,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="C82" t="b">
         <f t="shared" si="1"/>
@@ -9206,7 +9209,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="C87" t="b">
         <f t="shared" si="1"/>
@@ -10031,7 +10034,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156" s="5" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>
@@ -10044,49 +10047,49 @@
   <dimension ref="A1:H1172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="116.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>892</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>893</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>894</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>895</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="B2" s="6">
         <v>42765</v>
@@ -10098,18 +10101,18 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="F2" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="G2" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B3" s="6">
         <v>42745</v>
@@ -10121,15 +10124,15 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="F3" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B4" s="6">
         <v>42745</v>
@@ -10141,15 +10144,15 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="F4" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B5" s="6">
         <v>42746</v>
@@ -10161,15 +10164,15 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="F5" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B6" s="6">
         <v>42746</v>
@@ -10181,15 +10184,15 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="F6" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B7" s="6">
         <v>42747</v>
@@ -10201,15 +10204,15 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="F7" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B8" s="6">
         <v>42748</v>
@@ -10221,15 +10224,15 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="F8" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B9" s="6">
         <v>42755</v>
@@ -10241,15 +10244,15 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="F9" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B10" s="6">
         <v>42757</v>
@@ -10261,15 +10264,15 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="F10" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="B11" s="6">
         <v>42757</v>
@@ -10281,10 +10284,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="F11" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -10301,10 +10304,10 @@
         <v>657</v>
       </c>
       <c r="E12" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="F12" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>